<commit_message>
added inductance calculator with air gap to table
</commit_message>
<xml_diff>
--- a/documentation/DCDCv9-3_Table.xlsx
+++ b/documentation/DCDCv9-3_Table.xlsx
@@ -128,6 +128,11 @@
 https://jlcpcb.com/impedance</t>
       </text>
     </comment>
+    <comment authorId="0" ref="B27">
+      <text>
+        <t xml:space="preserve">Air gap is subtracted from the mag. length in the R_m calculation</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -164,7 +169,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3274" uniqueCount="790">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3287" uniqueCount="799">
   <si>
     <t>DCDCv9-3 Table</t>
   </si>
@@ -2391,6 +2396,33 @@
   </si>
   <si>
     <t>dead time</t>
+  </si>
+  <si>
+    <t>Inductance calculator with air gap</t>
+  </si>
+  <si>
+    <t>Mag. total length.</t>
+  </si>
+  <si>
+    <t>Air gap length</t>
+  </si>
+  <si>
+    <t>µ_r core</t>
+  </si>
+  <si>
+    <t>Cross-sectional area</t>
+  </si>
+  <si>
+    <t>Number of turns</t>
+  </si>
+  <si>
+    <t>Inductance</t>
+  </si>
+  <si>
+    <t>total R_m</t>
+  </si>
+  <si>
+    <t>H^-1</t>
   </si>
   <si>
     <t>Halfbridge FET Selection</t>
@@ -4182,7 +4214,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="449">
+  <cellXfs count="450">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -5444,6 +5476,9 @@
     <xf borderId="16" fillId="0" fontId="6" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="16" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -5719,11 +5754,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="2110666859"/>
-        <c:axId val="218758895"/>
+        <c:axId val="22909543"/>
+        <c:axId val="277121533"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2110666859"/>
+        <c:axId val="22909543"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5775,10 +5810,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="218758895"/>
+        <c:crossAx val="277121533"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="218758895"/>
+        <c:axId val="277121533"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5853,7 +5888,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2110666859"/>
+        <c:crossAx val="22909543"/>
         <c:majorUnit val="0.2"/>
         <c:minorUnit val="0.1"/>
       </c:valAx>
@@ -5955,11 +5990,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1577309081"/>
-        <c:axId val="1505710703"/>
+        <c:axId val="535757047"/>
+        <c:axId val="43241536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1577309081"/>
+        <c:axId val="535757047"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="52.0"/>
@@ -6012,10 +6047,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1505710703"/>
+        <c:crossAx val="43241536"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1505710703"/>
+        <c:axId val="43241536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6090,7 +6125,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1577309081"/>
+        <c:crossAx val="535757047"/>
         <c:majorUnit val="0.2"/>
         <c:minorUnit val="0.1"/>
       </c:valAx>
@@ -6689,130 +6724,130 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="7" t="s">
-        <v>617</v>
+        <v>626</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="7"/>
-      <c r="E1" s="427"/>
+      <c r="E1" s="428"/>
     </row>
     <row r="2">
-      <c r="A2" s="428" t="s">
-        <v>618</v>
-      </c>
-      <c r="B2" s="429">
+      <c r="A2" s="429" t="s">
+        <v>627</v>
+      </c>
+      <c r="B2" s="430">
         <v>600.0</v>
       </c>
-      <c r="C2" s="430" t="s">
+      <c r="C2" s="431" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="431" t="s">
-        <v>619</v>
+      <c r="A3" s="432" t="s">
+        <v>628</v>
       </c>
       <c r="B3" s="18">
         <v>4.0</v>
       </c>
-      <c r="C3" s="432" t="s">
-        <v>620</v>
+      <c r="C3" s="433" t="s">
+        <v>629</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="431" t="s">
-        <v>621</v>
+      <c r="A4" s="432" t="s">
+        <v>630</v>
       </c>
       <c r="B4" s="3">
         <v>150.0</v>
       </c>
-      <c r="C4" s="432" t="s">
+      <c r="C4" s="433" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="431" t="s">
-        <v>622</v>
+      <c r="A5" s="432" t="s">
+        <v>631</v>
       </c>
       <c r="B5" s="18">
         <v>4.0</v>
       </c>
-      <c r="C5" s="432" t="s">
+      <c r="C5" s="433" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="433" t="s">
-        <v>623</v>
-      </c>
-      <c r="B6" s="434">
+      <c r="A6" s="434" t="s">
+        <v>632</v>
+      </c>
+      <c r="B6" s="435">
         <v>0.5</v>
       </c>
-      <c r="C6" s="435" t="s">
-        <v>624</v>
+      <c r="C6" s="436" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="40" t="s">
-        <v>625</v>
+        <v>634</v>
       </c>
       <c r="B7" s="40" t="s">
-        <v>626</v>
+        <v>635</v>
       </c>
       <c r="C7" s="40" t="s">
-        <v>627</v>
+        <v>636</v>
       </c>
       <c r="D7" s="40" t="s">
-        <v>628</v>
+        <v>637</v>
       </c>
       <c r="E7" s="40" t="s">
-        <v>629</v>
+        <v>638</v>
       </c>
       <c r="F7" s="40" t="s">
-        <v>630</v>
+        <v>639</v>
       </c>
       <c r="G7" s="40" t="s">
-        <v>631</v>
+        <v>640</v>
       </c>
       <c r="H7" s="40" t="s">
-        <v>632</v>
+        <v>641</v>
       </c>
       <c r="I7" s="40" t="s">
-        <v>633</v>
+        <v>642</v>
       </c>
       <c r="J7" s="40" t="s">
-        <v>634</v>
+        <v>643</v>
       </c>
       <c r="K7" s="40" t="s">
-        <v>635</v>
+        <v>644</v>
       </c>
       <c r="L7" s="40" t="s">
-        <v>636</v>
+        <v>645</v>
       </c>
       <c r="M7" s="40" t="s">
-        <v>637</v>
-      </c>
-      <c r="N7" s="436"/>
-      <c r="O7" s="436"/>
-      <c r="P7" s="436"/>
-      <c r="Q7" s="436"/>
-      <c r="R7" s="436"/>
-      <c r="S7" s="436"/>
-      <c r="T7" s="436"/>
-      <c r="U7" s="436"/>
-      <c r="V7" s="436"/>
-      <c r="W7" s="436"/>
-      <c r="X7" s="436"/>
-      <c r="Y7" s="436"/>
-      <c r="Z7" s="436"/>
+        <v>646</v>
+      </c>
+      <c r="N7" s="437"/>
+      <c r="O7" s="437"/>
+      <c r="P7" s="437"/>
+      <c r="Q7" s="437"/>
+      <c r="R7" s="437"/>
+      <c r="S7" s="437"/>
+      <c r="T7" s="437"/>
+      <c r="U7" s="437"/>
+      <c r="V7" s="437"/>
+      <c r="W7" s="437"/>
+      <c r="X7" s="437"/>
+      <c r="Y7" s="437"/>
+      <c r="Z7" s="437"/>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>638</v>
-      </c>
-      <c r="B8" s="437" t="s">
-        <v>639</v>
-      </c>
-      <c r="C8" s="438">
+        <v>647</v>
+      </c>
+      <c r="B8" s="438" t="s">
+        <v>648</v>
+      </c>
+      <c r="C8" s="439">
         <v>41.11</v>
       </c>
       <c r="D8" s="43">
@@ -6828,19 +6863,19 @@
         <f t="shared" ref="G8:G35" si="1">D8*E8</f>
         <v>454.4</v>
       </c>
-      <c r="H8" s="439">
+      <c r="H8" s="440">
         <f t="shared" ref="H8:H35" si="2">D8/1000*$B$3^2</f>
         <v>0.512</v>
       </c>
-      <c r="I8" s="439">
+      <c r="I8" s="440">
         <f t="shared" ref="I8:I35" si="3">($B$2*$B$3*$B$4*1000*(E8*10^-9)/$B$5)*$B$6</f>
         <v>0.639</v>
       </c>
-      <c r="J8" s="439">
+      <c r="J8" s="440">
         <f t="shared" ref="J8:J35" si="4">F8*10^-9*$B$2*$B$4*1000</f>
         <v>0</v>
       </c>
-      <c r="K8" s="439">
+      <c r="K8" s="440">
         <f t="shared" ref="K8:K35" si="5">H8+I8+J8</f>
         <v>1.151</v>
       </c>
@@ -6855,12 +6890,12 @@
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>640</v>
-      </c>
-      <c r="B9" s="440" t="s">
-        <v>641</v>
-      </c>
-      <c r="C9" s="438">
+        <v>649</v>
+      </c>
+      <c r="B9" s="441" t="s">
+        <v>650</v>
+      </c>
+      <c r="C9" s="439">
         <v>13.32</v>
       </c>
       <c r="D9" s="43">
@@ -6876,19 +6911,19 @@
         <f t="shared" si="1"/>
         <v>406</v>
       </c>
-      <c r="H9" s="439">
+      <c r="H9" s="440">
         <f t="shared" si="2"/>
         <v>1.12</v>
       </c>
-      <c r="I9" s="439">
+      <c r="I9" s="440">
         <f t="shared" si="3"/>
         <v>0.261</v>
       </c>
-      <c r="J9" s="439">
+      <c r="J9" s="440">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K9" s="439">
+      <c r="K9" s="440">
         <f t="shared" si="5"/>
         <v>1.381</v>
       </c>
@@ -6903,12 +6938,12 @@
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>642</v>
-      </c>
-      <c r="B10" s="440" t="s">
-        <v>643</v>
-      </c>
-      <c r="C10" s="438">
+        <v>651</v>
+      </c>
+      <c r="B10" s="441" t="s">
+        <v>652</v>
+      </c>
+      <c r="C10" s="439">
         <v>12.8</v>
       </c>
       <c r="D10" s="43">
@@ -6924,19 +6959,19 @@
         <f t="shared" si="1"/>
         <v>429</v>
       </c>
-      <c r="H10" s="439">
+      <c r="H10" s="440">
         <f t="shared" si="2"/>
         <v>2.08</v>
       </c>
-      <c r="I10" s="439">
+      <c r="I10" s="440">
         <f t="shared" si="3"/>
         <v>0.1485</v>
       </c>
-      <c r="J10" s="439">
+      <c r="J10" s="440">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K10" s="439">
+      <c r="K10" s="440">
         <f t="shared" si="5"/>
         <v>2.2285</v>
       </c>
@@ -6951,12 +6986,12 @@
     </row>
     <row r="11">
       <c r="A11" s="7" t="s">
-        <v>644</v>
-      </c>
-      <c r="B11" s="437" t="s">
-        <v>645</v>
-      </c>
-      <c r="C11" s="438">
+        <v>653</v>
+      </c>
+      <c r="B11" s="438" t="s">
+        <v>654</v>
+      </c>
+      <c r="C11" s="439">
         <v>8.3</v>
       </c>
       <c r="D11" s="43">
@@ -6972,19 +7007,19 @@
         <f t="shared" si="1"/>
         <v>1364</v>
       </c>
-      <c r="H11" s="439">
+      <c r="H11" s="440">
         <f t="shared" si="2"/>
         <v>0.992</v>
       </c>
-      <c r="I11" s="439">
+      <c r="I11" s="440">
         <f t="shared" si="3"/>
         <v>0.99</v>
       </c>
-      <c r="J11" s="439">
+      <c r="J11" s="440">
         <f t="shared" si="4"/>
         <v>3.96</v>
       </c>
-      <c r="K11" s="439">
+      <c r="K11" s="440">
         <f t="shared" si="5"/>
         <v>5.942</v>
       </c>
@@ -6999,12 +7034,12 @@
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>646</v>
-      </c>
-      <c r="B12" s="437" t="s">
-        <v>647</v>
-      </c>
-      <c r="C12" s="438">
+        <v>655</v>
+      </c>
+      <c r="B12" s="438" t="s">
+        <v>656</v>
+      </c>
+      <c r="C12" s="439">
         <v>10.25</v>
       </c>
       <c r="D12" s="43">
@@ -7020,19 +7055,19 @@
         <f t="shared" si="1"/>
         <v>1372</v>
       </c>
-      <c r="H12" s="439">
+      <c r="H12" s="440">
         <f t="shared" si="2"/>
         <v>0.784</v>
       </c>
-      <c r="I12" s="439">
+      <c r="I12" s="440">
         <f t="shared" si="3"/>
         <v>1.26</v>
       </c>
-      <c r="J12" s="439">
+      <c r="J12" s="440">
         <f t="shared" si="4"/>
         <v>5.04</v>
       </c>
-      <c r="K12" s="439">
+      <c r="K12" s="440">
         <f t="shared" si="5"/>
         <v>7.084</v>
       </c>
@@ -7047,12 +7082,12 @@
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>648</v>
-      </c>
-      <c r="B13" s="440" t="s">
-        <v>649</v>
-      </c>
-      <c r="C13" s="438">
+        <v>657</v>
+      </c>
+      <c r="B13" s="441" t="s">
+        <v>658</v>
+      </c>
+      <c r="C13" s="439">
         <v>5.59</v>
       </c>
       <c r="D13" s="43">
@@ -7068,19 +7103,19 @@
         <f t="shared" si="1"/>
         <v>2184</v>
       </c>
-      <c r="H13" s="439">
+      <c r="H13" s="440">
         <f t="shared" si="2"/>
         <v>2.912</v>
       </c>
-      <c r="I13" s="439">
+      <c r="I13" s="440">
         <f t="shared" si="3"/>
         <v>0.54</v>
       </c>
-      <c r="J13" s="439">
+      <c r="J13" s="440">
         <f t="shared" si="4"/>
         <v>4.14</v>
       </c>
-      <c r="K13" s="439">
+      <c r="K13" s="440">
         <f t="shared" si="5"/>
         <v>7.592</v>
       </c>
@@ -7095,12 +7130,12 @@
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>650</v>
-      </c>
-      <c r="B14" s="437" t="s">
-        <v>651</v>
-      </c>
-      <c r="C14" s="438">
+        <v>659</v>
+      </c>
+      <c r="B14" s="438" t="s">
+        <v>660</v>
+      </c>
+      <c r="C14" s="439">
         <v>8.15</v>
       </c>
       <c r="D14" s="43">
@@ -7116,19 +7151,19 @@
         <f t="shared" si="1"/>
         <v>1955</v>
       </c>
-      <c r="H14" s="439">
+      <c r="H14" s="440">
         <f t="shared" si="2"/>
         <v>1.36</v>
       </c>
-      <c r="I14" s="439">
+      <c r="I14" s="440">
         <f t="shared" si="3"/>
         <v>1.035</v>
       </c>
-      <c r="J14" s="439">
+      <c r="J14" s="440">
         <f t="shared" si="4"/>
         <v>6.21</v>
       </c>
-      <c r="K14" s="439">
+      <c r="K14" s="440">
         <f t="shared" si="5"/>
         <v>8.605</v>
       </c>
@@ -7143,12 +7178,12 @@
     </row>
     <row r="15">
       <c r="A15" s="7" t="s">
-        <v>652</v>
-      </c>
-      <c r="B15" s="440" t="s">
-        <v>653</v>
-      </c>
-      <c r="C15" s="438">
+        <v>661</v>
+      </c>
+      <c r="B15" s="441" t="s">
+        <v>662</v>
+      </c>
+      <c r="C15" s="439">
         <v>7.38</v>
       </c>
       <c r="D15" s="43">
@@ -7164,19 +7199,19 @@
         <f t="shared" si="1"/>
         <v>2797.2</v>
       </c>
-      <c r="H15" s="439">
+      <c r="H15" s="440">
         <f t="shared" si="2"/>
         <v>1.184</v>
       </c>
-      <c r="I15" s="439">
+      <c r="I15" s="440">
         <f t="shared" si="3"/>
         <v>1.701</v>
       </c>
-      <c r="J15" s="439">
+      <c r="J15" s="440">
         <f t="shared" si="4"/>
         <v>6.93</v>
       </c>
-      <c r="K15" s="439">
+      <c r="K15" s="440">
         <f t="shared" si="5"/>
         <v>9.815</v>
       </c>
@@ -7191,12 +7226,12 @@
     </row>
     <row r="16">
       <c r="A16" s="7" t="s">
-        <v>654</v>
-      </c>
-      <c r="B16" s="440" t="s">
-        <v>655</v>
-      </c>
-      <c r="C16" s="438">
+        <v>663</v>
+      </c>
+      <c r="B16" s="441" t="s">
+        <v>664</v>
+      </c>
+      <c r="C16" s="439">
         <v>10.16</v>
       </c>
       <c r="D16" s="43">
@@ -7212,19 +7247,19 @@
         <f t="shared" si="1"/>
         <v>2112</v>
       </c>
-      <c r="H16" s="439">
+      <c r="H16" s="440">
         <f t="shared" si="2"/>
         <v>1.024</v>
       </c>
-      <c r="I16" s="439">
+      <c r="I16" s="440">
         <f t="shared" si="3"/>
         <v>1.485</v>
       </c>
-      <c r="J16" s="439">
+      <c r="J16" s="440">
         <f t="shared" si="4"/>
         <v>7.38</v>
       </c>
-      <c r="K16" s="439">
+      <c r="K16" s="440">
         <f t="shared" si="5"/>
         <v>9.889</v>
       </c>
@@ -7239,12 +7274,12 @@
     </row>
     <row r="17">
       <c r="A17" s="3" t="s">
-        <v>656</v>
-      </c>
-      <c r="B17" s="437" t="s">
-        <v>657</v>
-      </c>
-      <c r="C17" s="438">
+        <v>665</v>
+      </c>
+      <c r="B17" s="438" t="s">
+        <v>666</v>
+      </c>
+      <c r="C17" s="439">
         <v>9.95</v>
       </c>
       <c r="D17" s="43">
@@ -7260,19 +7295,19 @@
         <f t="shared" si="1"/>
         <v>1920</v>
       </c>
-      <c r="H17" s="439">
+      <c r="H17" s="440">
         <f t="shared" si="2"/>
         <v>1.28</v>
       </c>
-      <c r="I17" s="439">
+      <c r="I17" s="440">
         <f t="shared" si="3"/>
         <v>1.08</v>
       </c>
-      <c r="J17" s="439">
+      <c r="J17" s="440">
         <f t="shared" si="4"/>
         <v>7.65</v>
       </c>
-      <c r="K17" s="439">
+      <c r="K17" s="440">
         <f t="shared" si="5"/>
         <v>10.01</v>
       </c>
@@ -7287,12 +7322,12 @@
     </row>
     <row r="18">
       <c r="A18" s="3" t="s">
-        <v>658</v>
-      </c>
-      <c r="B18" s="437" t="s">
-        <v>659</v>
-      </c>
-      <c r="C18" s="441">
+        <v>667</v>
+      </c>
+      <c r="B18" s="438" t="s">
+        <v>668</v>
+      </c>
+      <c r="C18" s="442">
         <v>15.41</v>
       </c>
       <c r="D18" s="43">
@@ -7308,23 +7343,23 @@
         <f t="shared" si="1"/>
         <v>1096.2</v>
       </c>
-      <c r="H18" s="442">
+      <c r="H18" s="443">
         <f t="shared" si="2"/>
         <v>0.464</v>
       </c>
-      <c r="I18" s="442">
+      <c r="I18" s="443">
         <f t="shared" si="3"/>
         <v>1.701</v>
       </c>
-      <c r="J18" s="442">
+      <c r="J18" s="443">
         <f t="shared" si="4"/>
         <v>9.45</v>
       </c>
-      <c r="K18" s="442">
+      <c r="K18" s="443">
         <f t="shared" si="5"/>
         <v>11.615</v>
       </c>
-      <c r="L18" s="443">
+      <c r="L18" s="444">
         <f t="shared" si="6"/>
         <v>2.165</v>
       </c>
@@ -7335,12 +7370,12 @@
     </row>
     <row r="19">
       <c r="A19" s="3" t="s">
-        <v>660</v>
-      </c>
-      <c r="B19" s="437" t="s">
-        <v>661</v>
-      </c>
-      <c r="C19" s="438">
+        <v>669</v>
+      </c>
+      <c r="B19" s="438" t="s">
+        <v>670</v>
+      </c>
+      <c r="C19" s="439">
         <v>16.16</v>
       </c>
       <c r="D19" s="43">
@@ -7356,19 +7391,19 @@
         <f t="shared" si="1"/>
         <v>1368</v>
       </c>
-      <c r="H19" s="439">
+      <c r="H19" s="440">
         <f t="shared" si="2"/>
         <v>0.384</v>
       </c>
-      <c r="I19" s="439">
+      <c r="I19" s="440">
         <f t="shared" si="3"/>
         <v>2.565</v>
       </c>
-      <c r="J19" s="439">
+      <c r="J19" s="440">
         <f t="shared" si="4"/>
         <v>9.9</v>
       </c>
-      <c r="K19" s="439">
+      <c r="K19" s="440">
         <f t="shared" si="5"/>
         <v>12.849</v>
       </c>
@@ -7383,12 +7418,12 @@
     </row>
     <row r="20">
       <c r="A20" s="3" t="s">
-        <v>662</v>
-      </c>
-      <c r="B20" s="440" t="s">
-        <v>663</v>
-      </c>
-      <c r="C20" s="438">
+        <v>671</v>
+      </c>
+      <c r="B20" s="441" t="s">
+        <v>672</v>
+      </c>
+      <c r="C20" s="439">
         <v>6.37</v>
       </c>
       <c r="D20" s="43">
@@ -7404,19 +7439,19 @@
         <f t="shared" si="1"/>
         <v>2763.6</v>
       </c>
-      <c r="H20" s="439">
+      <c r="H20" s="440">
         <f t="shared" si="2"/>
         <v>4.704</v>
       </c>
-      <c r="I20" s="439">
+      <c r="I20" s="440">
         <f t="shared" si="3"/>
         <v>0.423</v>
       </c>
-      <c r="J20" s="439">
+      <c r="J20" s="440">
         <f t="shared" si="4"/>
         <v>6.75</v>
       </c>
-      <c r="K20" s="439">
+      <c r="K20" s="440">
         <f t="shared" si="5"/>
         <v>11.877</v>
       </c>
@@ -7431,12 +7466,12 @@
     </row>
     <row r="21">
       <c r="A21" s="3" t="s">
-        <v>664</v>
-      </c>
-      <c r="B21" s="437" t="s">
-        <v>665</v>
-      </c>
-      <c r="C21" s="441">
+        <v>673</v>
+      </c>
+      <c r="B21" s="438" t="s">
+        <v>674</v>
+      </c>
+      <c r="C21" s="442">
         <v>16.17</v>
       </c>
       <c r="D21" s="43">
@@ -7452,19 +7487,19 @@
         <f t="shared" si="1"/>
         <v>4530</v>
       </c>
-      <c r="H21" s="439">
+      <c r="H21" s="440">
         <f t="shared" si="2"/>
         <v>0.48</v>
       </c>
-      <c r="I21" s="439">
+      <c r="I21" s="440">
         <f t="shared" si="3"/>
         <v>6.795</v>
       </c>
-      <c r="J21" s="439">
+      <c r="J21" s="440">
         <f t="shared" si="4"/>
         <v>12.42</v>
       </c>
-      <c r="K21" s="439">
+      <c r="K21" s="440">
         <f t="shared" si="5"/>
         <v>19.695</v>
       </c>
@@ -7479,12 +7514,12 @@
     </row>
     <row r="22">
       <c r="A22" s="3" t="s">
-        <v>666</v>
-      </c>
-      <c r="B22" s="440" t="s">
-        <v>667</v>
-      </c>
-      <c r="C22" s="438">
+        <v>675</v>
+      </c>
+      <c r="B22" s="441" t="s">
+        <v>676</v>
+      </c>
+      <c r="C22" s="439">
         <v>12.31</v>
       </c>
       <c r="D22" s="43">
@@ -7500,19 +7535,19 @@
         <f t="shared" si="1"/>
         <v>2088</v>
       </c>
-      <c r="H22" s="439">
+      <c r="H22" s="440">
         <f t="shared" si="2"/>
         <v>1.152</v>
       </c>
-      <c r="I22" s="439">
+      <c r="I22" s="440">
         <f t="shared" si="3"/>
         <v>1.305</v>
       </c>
-      <c r="J22" s="439">
+      <c r="J22" s="440">
         <f t="shared" si="4"/>
         <v>11.88</v>
       </c>
-      <c r="K22" s="439">
+      <c r="K22" s="440">
         <f t="shared" si="5"/>
         <v>14.337</v>
       </c>
@@ -7527,12 +7562,12 @@
     </row>
     <row r="23">
       <c r="A23" s="3" t="s">
-        <v>668</v>
-      </c>
-      <c r="B23" s="440" t="s">
-        <v>669</v>
-      </c>
-      <c r="C23" s="438">
+        <v>677</v>
+      </c>
+      <c r="B23" s="441" t="s">
+        <v>678</v>
+      </c>
+      <c r="C23" s="439">
         <v>5.82</v>
       </c>
       <c r="D23" s="43">
@@ -7548,19 +7583,19 @@
         <f t="shared" si="1"/>
         <v>2761.2</v>
       </c>
-      <c r="H23" s="439">
+      <c r="H23" s="440">
         <f t="shared" si="2"/>
         <v>7.488</v>
       </c>
-      <c r="I23" s="439">
+      <c r="I23" s="440">
         <f t="shared" si="3"/>
         <v>0.2655</v>
       </c>
-      <c r="J23" s="439">
+      <c r="J23" s="440">
         <f t="shared" si="4"/>
         <v>5.58</v>
       </c>
-      <c r="K23" s="439">
+      <c r="K23" s="440">
         <f t="shared" si="5"/>
         <v>13.3335</v>
       </c>
@@ -7575,12 +7610,12 @@
     </row>
     <row r="24">
       <c r="A24" s="3" t="s">
-        <v>670</v>
-      </c>
-      <c r="B24" s="437" t="s">
-        <v>671</v>
-      </c>
-      <c r="C24" s="438">
+        <v>679</v>
+      </c>
+      <c r="B24" s="438" t="s">
+        <v>680</v>
+      </c>
+      <c r="C24" s="439">
         <v>9.58</v>
       </c>
       <c r="D24" s="43">
@@ -7596,19 +7631,19 @@
         <f t="shared" si="1"/>
         <v>2875</v>
       </c>
-      <c r="H24" s="439">
+      <c r="H24" s="440">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="I24" s="439">
+      <c r="I24" s="440">
         <f t="shared" si="3"/>
         <v>1.035</v>
       </c>
-      <c r="J24" s="439">
+      <c r="J24" s="440">
         <f t="shared" si="4"/>
         <v>11.43</v>
       </c>
-      <c r="K24" s="439">
+      <c r="K24" s="440">
         <f t="shared" si="5"/>
         <v>14.465</v>
       </c>
@@ -7623,12 +7658,12 @@
     </row>
     <row r="25">
       <c r="A25" s="3" t="s">
-        <v>672</v>
-      </c>
-      <c r="B25" s="437" t="s">
-        <v>673</v>
-      </c>
-      <c r="C25" s="438">
+        <v>681</v>
+      </c>
+      <c r="B25" s="438" t="s">
+        <v>682</v>
+      </c>
+      <c r="C25" s="439">
         <v>10.78</v>
       </c>
       <c r="D25" s="43">
@@ -7644,19 +7679,19 @@
         <f t="shared" si="1"/>
         <v>2822</v>
       </c>
-      <c r="H25" s="439">
+      <c r="H25" s="440">
         <f t="shared" si="2"/>
         <v>1.328</v>
       </c>
-      <c r="I25" s="439">
+      <c r="I25" s="440">
         <f t="shared" si="3"/>
         <v>1.53</v>
       </c>
-      <c r="J25" s="439">
+      <c r="J25" s="440">
         <f t="shared" si="4"/>
         <v>14.85</v>
       </c>
-      <c r="K25" s="439">
+      <c r="K25" s="440">
         <f t="shared" si="5"/>
         <v>17.708</v>
       </c>
@@ -7671,12 +7706,12 @@
     </row>
     <row r="26">
       <c r="A26" s="3" t="s">
-        <v>674</v>
-      </c>
-      <c r="B26" s="437" t="s">
-        <v>675</v>
-      </c>
-      <c r="C26" s="441">
+        <v>683</v>
+      </c>
+      <c r="B26" s="438" t="s">
+        <v>684</v>
+      </c>
+      <c r="C26" s="442">
         <v>21.16</v>
       </c>
       <c r="D26" s="43">
@@ -7692,19 +7727,19 @@
         <f t="shared" si="1"/>
         <v>869.4</v>
       </c>
-      <c r="H26" s="439">
+      <c r="H26" s="440">
         <f t="shared" si="2"/>
         <v>0.368</v>
       </c>
-      <c r="I26" s="439">
+      <c r="I26" s="440">
         <f t="shared" si="3"/>
         <v>1.701</v>
       </c>
-      <c r="J26" s="439">
+      <c r="J26" s="440">
         <f t="shared" si="4"/>
         <v>23.76</v>
       </c>
-      <c r="K26" s="439">
+      <c r="K26" s="440">
         <f t="shared" si="5"/>
         <v>25.829</v>
       </c>
@@ -7719,12 +7754,12 @@
     </row>
     <row r="27">
       <c r="A27" s="3" t="s">
-        <v>676</v>
-      </c>
-      <c r="B27" s="437" t="s">
-        <v>677</v>
-      </c>
-      <c r="C27" s="438">
+        <v>685</v>
+      </c>
+      <c r="B27" s="438" t="s">
+        <v>686</v>
+      </c>
+      <c r="C27" s="439">
         <v>18.99</v>
       </c>
       <c r="D27" s="43">
@@ -7740,19 +7775,19 @@
         <f t="shared" si="1"/>
         <v>2583</v>
       </c>
-      <c r="H27" s="439">
+      <c r="H27" s="440">
         <f t="shared" si="2"/>
         <v>0.656</v>
       </c>
-      <c r="I27" s="439">
+      <c r="I27" s="440">
         <f t="shared" si="3"/>
         <v>2.835</v>
       </c>
-      <c r="J27" s="439">
+      <c r="J27" s="440">
         <f t="shared" si="4"/>
         <v>27</v>
       </c>
-      <c r="K27" s="439">
+      <c r="K27" s="440">
         <f t="shared" si="5"/>
         <v>30.491</v>
       </c>
@@ -7767,10 +7802,10 @@
     </row>
     <row r="28">
       <c r="A28" s="3" t="s">
-        <v>678</v>
-      </c>
-      <c r="B28" s="437" t="s">
-        <v>679</v>
+        <v>687</v>
+      </c>
+      <c r="B28" s="438" t="s">
+        <v>688</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>315</v>
@@ -7788,19 +7823,19 @@
         <f t="shared" si="1"/>
         <v>4606</v>
       </c>
-      <c r="H28" s="439">
+      <c r="H28" s="440">
         <f t="shared" si="2"/>
         <v>0.224</v>
       </c>
-      <c r="I28" s="439">
+      <c r="I28" s="440">
         <f t="shared" si="3"/>
         <v>14.805</v>
       </c>
-      <c r="J28" s="439">
+      <c r="J28" s="440">
         <f t="shared" si="4"/>
         <v>29.88</v>
       </c>
-      <c r="K28" s="439">
+      <c r="K28" s="440">
         <f t="shared" si="5"/>
         <v>44.909</v>
       </c>
@@ -7815,12 +7850,12 @@
     </row>
     <row r="29">
       <c r="A29" s="3" t="s">
-        <v>680</v>
-      </c>
-      <c r="B29" s="440" t="s">
-        <v>681</v>
-      </c>
-      <c r="C29" s="438">
+        <v>689</v>
+      </c>
+      <c r="B29" s="441" t="s">
+        <v>690</v>
+      </c>
+      <c r="C29" s="439">
         <v>35.41</v>
       </c>
       <c r="D29" s="43">
@@ -7836,19 +7871,19 @@
         <f t="shared" si="1"/>
         <v>1521.5</v>
       </c>
-      <c r="H29" s="439">
+      <c r="H29" s="440">
         <f t="shared" si="2"/>
         <v>0.136</v>
       </c>
-      <c r="I29" s="439">
+      <c r="I29" s="440">
         <f t="shared" si="3"/>
         <v>8.055</v>
       </c>
-      <c r="J29" s="439">
+      <c r="J29" s="440">
         <f t="shared" si="4"/>
         <v>32.58</v>
       </c>
-      <c r="K29" s="439">
+      <c r="K29" s="440">
         <f t="shared" si="5"/>
         <v>40.771</v>
       </c>
@@ -7863,12 +7898,12 @@
     </row>
     <row r="30">
       <c r="A30" s="3" t="s">
-        <v>682</v>
-      </c>
-      <c r="B30" s="440" t="s">
-        <v>683</v>
-      </c>
-      <c r="C30" s="438">
+        <v>691</v>
+      </c>
+      <c r="B30" s="441" t="s">
+        <v>692</v>
+      </c>
+      <c r="C30" s="439">
         <v>5.69</v>
       </c>
       <c r="D30" s="43">
@@ -7884,19 +7919,19 @@
         <f t="shared" si="1"/>
         <v>6270</v>
       </c>
-      <c r="H30" s="439">
+      <c r="H30" s="440">
         <f t="shared" si="2"/>
         <v>1.52</v>
       </c>
-      <c r="I30" s="439">
+      <c r="I30" s="440">
         <f t="shared" si="3"/>
         <v>2.97</v>
       </c>
-      <c r="J30" s="439">
+      <c r="J30" s="440">
         <f t="shared" si="4"/>
         <v>33.48</v>
       </c>
-      <c r="K30" s="439">
+      <c r="K30" s="440">
         <f t="shared" si="5"/>
         <v>37.97</v>
       </c>
@@ -7911,12 +7946,12 @@
     </row>
     <row r="31">
       <c r="A31" s="3" t="s">
-        <v>684</v>
-      </c>
-      <c r="B31" s="440" t="s">
-        <v>685</v>
-      </c>
-      <c r="C31" s="441">
+        <v>693</v>
+      </c>
+      <c r="B31" s="441" t="s">
+        <v>694</v>
+      </c>
+      <c r="C31" s="442">
         <v>34.44</v>
       </c>
       <c r="D31" s="43">
@@ -7932,19 +7967,19 @@
         <f t="shared" si="1"/>
         <v>1501.5</v>
       </c>
-      <c r="H31" s="439">
+      <c r="H31" s="440">
         <f t="shared" si="2"/>
         <v>0.1232</v>
       </c>
-      <c r="I31" s="439">
+      <c r="I31" s="440">
         <f t="shared" si="3"/>
         <v>8.775</v>
       </c>
-      <c r="J31" s="439">
+      <c r="J31" s="440">
         <f t="shared" si="4"/>
         <v>76.5</v>
       </c>
-      <c r="K31" s="439">
+      <c r="K31" s="440">
         <f t="shared" si="5"/>
         <v>85.3982</v>
       </c>
@@ -7959,12 +7994,12 @@
     </row>
     <row r="32">
       <c r="A32" s="3" t="s">
-        <v>686</v>
-      </c>
-      <c r="B32" s="437" t="s">
-        <v>687</v>
-      </c>
-      <c r="C32" s="438">
+        <v>695</v>
+      </c>
+      <c r="B32" s="438" t="s">
+        <v>696</v>
+      </c>
+      <c r="C32" s="439">
         <v>0.846</v>
       </c>
       <c r="D32" s="43">
@@ -7980,19 +8015,19 @@
         <f t="shared" si="1"/>
         <v>4920</v>
       </c>
-      <c r="H32" s="439">
+      <c r="H32" s="440">
         <f t="shared" si="2"/>
         <v>4.8</v>
       </c>
-      <c r="I32" s="439">
+      <c r="I32" s="440">
         <f t="shared" si="3"/>
         <v>0.738</v>
       </c>
-      <c r="J32" s="439">
+      <c r="J32" s="440">
         <f t="shared" si="4"/>
         <v>90</v>
       </c>
-      <c r="K32" s="439">
+      <c r="K32" s="440">
         <f t="shared" si="5"/>
         <v>95.538</v>
       </c>
@@ -8007,12 +8042,12 @@
     </row>
     <row r="33">
       <c r="A33" s="3" t="s">
-        <v>688</v>
-      </c>
-      <c r="B33" s="437" t="s">
-        <v>689</v>
-      </c>
-      <c r="C33" s="438">
+        <v>697</v>
+      </c>
+      <c r="B33" s="438" t="s">
+        <v>698</v>
+      </c>
+      <c r="C33" s="439">
         <v>5.86</v>
       </c>
       <c r="D33" s="43">
@@ -8022,25 +8057,25 @@
         <v>11.0</v>
       </c>
       <c r="F33" s="43" t="s">
-        <v>690</v>
+        <v>699</v>
       </c>
       <c r="G33" s="25">
         <f t="shared" si="1"/>
         <v>4950</v>
       </c>
-      <c r="H33" s="439">
+      <c r="H33" s="440">
         <f t="shared" si="2"/>
         <v>7.2</v>
       </c>
-      <c r="I33" s="439">
+      <c r="I33" s="440">
         <f t="shared" si="3"/>
         <v>0.495</v>
       </c>
-      <c r="J33" s="439" t="str">
+      <c r="J33" s="440" t="str">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K33" s="439" t="str">
+      <c r="K33" s="440" t="str">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
@@ -8055,12 +8090,12 @@
     </row>
     <row r="34">
       <c r="A34" s="3" t="s">
-        <v>691</v>
-      </c>
-      <c r="B34" s="437" t="s">
-        <v>692</v>
-      </c>
-      <c r="C34" s="438">
+        <v>700</v>
+      </c>
+      <c r="B34" s="438" t="s">
+        <v>701</v>
+      </c>
+      <c r="C34" s="439">
         <v>6.45</v>
       </c>
       <c r="D34" s="43">
@@ -8070,25 +8105,25 @@
         <v>11.0</v>
       </c>
       <c r="F34" s="43" t="s">
-        <v>690</v>
+        <v>699</v>
       </c>
       <c r="G34" s="25">
         <f t="shared" si="1"/>
         <v>8250</v>
       </c>
-      <c r="H34" s="439">
+      <c r="H34" s="440">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="I34" s="439">
+      <c r="I34" s="440">
         <f t="shared" si="3"/>
         <v>0.495</v>
       </c>
-      <c r="J34" s="439" t="str">
+      <c r="J34" s="440" t="str">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K34" s="439" t="str">
+      <c r="K34" s="440" t="str">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
@@ -8103,12 +8138,12 @@
     </row>
     <row r="35">
       <c r="A35" s="3" t="s">
-        <v>693</v>
-      </c>
-      <c r="B35" s="440" t="s">
-        <v>694</v>
-      </c>
-      <c r="C35" s="438">
+        <v>702</v>
+      </c>
+      <c r="B35" s="441" t="s">
+        <v>703</v>
+      </c>
+      <c r="C35" s="439">
         <v>4.58</v>
       </c>
       <c r="D35" s="43">
@@ -8118,25 +8153,25 @@
         <v>5.0</v>
       </c>
       <c r="F35" s="43" t="s">
-        <v>690</v>
+        <v>699</v>
       </c>
       <c r="G35" s="25">
         <f t="shared" si="1"/>
         <v>5000</v>
       </c>
-      <c r="H35" s="439">
+      <c r="H35" s="440">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="I35" s="439">
+      <c r="I35" s="440">
         <f t="shared" si="3"/>
         <v>0.225</v>
       </c>
-      <c r="J35" s="439" t="str">
+      <c r="J35" s="440" t="str">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K35" s="439" t="str">
+      <c r="K35" s="440" t="str">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
@@ -8150,72 +8185,72 @@
       </c>
     </row>
     <row r="36">
-      <c r="B36" s="444"/>
+      <c r="B36" s="445"/>
     </row>
     <row r="37">
-      <c r="B37" s="444"/>
+      <c r="B37" s="445"/>
     </row>
     <row r="38">
       <c r="A38" s="7" t="s">
-        <v>695</v>
+        <v>704</v>
       </c>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="7"/>
     </row>
     <row r="39">
-      <c r="A39" s="428" t="s">
-        <v>618</v>
-      </c>
-      <c r="B39" s="429">
+      <c r="A39" s="429" t="s">
+        <v>627</v>
+      </c>
+      <c r="B39" s="430">
         <v>1.0</v>
       </c>
-      <c r="C39" s="430" t="s">
+      <c r="C39" s="431" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="431" t="s">
-        <v>619</v>
+      <c r="A40" s="432" t="s">
+        <v>628</v>
       </c>
       <c r="B40" s="3">
         <v>30.0</v>
       </c>
-      <c r="C40" s="432" t="s">
-        <v>620</v>
+      <c r="C40" s="433" t="s">
+        <v>629</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="431" t="s">
-        <v>621</v>
+      <c r="A41" s="432" t="s">
+        <v>630</v>
       </c>
       <c r="B41" s="3">
         <v>190.0</v>
       </c>
-      <c r="C41" s="432" t="s">
+      <c r="C41" s="433" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="431" t="s">
-        <v>622</v>
+      <c r="A42" s="432" t="s">
+        <v>631</v>
       </c>
       <c r="B42" s="18">
         <v>4.0</v>
       </c>
-      <c r="C42" s="432" t="s">
+      <c r="C42" s="433" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="433" t="s">
-        <v>623</v>
-      </c>
-      <c r="B43" s="434">
+      <c r="A43" s="434" t="s">
+        <v>632</v>
+      </c>
+      <c r="B43" s="435">
         <v>0.5</v>
       </c>
-      <c r="C43" s="435" t="s">
-        <v>624</v>
+      <c r="C43" s="436" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="44">
@@ -8225,79 +8260,79 @@
     </row>
     <row r="45">
       <c r="A45" s="40" t="s">
-        <v>625</v>
+        <v>634</v>
       </c>
       <c r="B45" s="40" t="s">
-        <v>626</v>
+        <v>635</v>
       </c>
       <c r="C45" s="40" t="s">
-        <v>627</v>
+        <v>636</v>
       </c>
       <c r="D45" s="40" t="s">
-        <v>696</v>
+        <v>705</v>
       </c>
       <c r="E45" s="40" t="s">
-        <v>697</v>
+        <v>706</v>
       </c>
       <c r="F45" s="40" t="s">
-        <v>698</v>
+        <v>707</v>
       </c>
       <c r="G45" s="40" t="s">
-        <v>699</v>
+        <v>708</v>
       </c>
       <c r="H45" s="40" t="s">
-        <v>700</v>
+        <v>709</v>
       </c>
       <c r="I45" s="40" t="s">
-        <v>628</v>
+        <v>637</v>
       </c>
       <c r="J45" s="40" t="s">
-        <v>629</v>
+        <v>638</v>
       </c>
       <c r="K45" s="40" t="s">
-        <v>630</v>
+        <v>639</v>
       </c>
       <c r="L45" s="40" t="s">
-        <v>631</v>
-      </c>
-      <c r="M45" s="445" t="s">
-        <v>632</v>
-      </c>
-      <c r="N45" s="445" t="s">
-        <v>633</v>
-      </c>
-      <c r="O45" s="445" t="s">
-        <v>634</v>
-      </c>
-      <c r="P45" s="445" t="s">
-        <v>635</v>
-      </c>
-      <c r="Q45" s="436"/>
-      <c r="R45" s="436"/>
-      <c r="S45" s="436"/>
-      <c r="T45" s="436"/>
-      <c r="U45" s="436"/>
-      <c r="V45" s="436"/>
-      <c r="W45" s="436"/>
-      <c r="X45" s="436"/>
-      <c r="Y45" s="436"/>
-      <c r="Z45" s="436"/>
+        <v>640</v>
+      </c>
+      <c r="M45" s="446" t="s">
+        <v>641</v>
+      </c>
+      <c r="N45" s="446" t="s">
+        <v>642</v>
+      </c>
+      <c r="O45" s="446" t="s">
+        <v>643</v>
+      </c>
+      <c r="P45" s="446" t="s">
+        <v>644</v>
+      </c>
+      <c r="Q45" s="437"/>
+      <c r="R45" s="437"/>
+      <c r="S45" s="437"/>
+      <c r="T45" s="437"/>
+      <c r="U45" s="437"/>
+      <c r="V45" s="437"/>
+      <c r="W45" s="437"/>
+      <c r="X45" s="437"/>
+      <c r="Y45" s="437"/>
+      <c r="Z45" s="437"/>
     </row>
     <row r="46">
       <c r="A46" s="3" t="s">
-        <v>701</v>
-      </c>
-      <c r="B46" s="446" t="s">
-        <v>702</v>
-      </c>
-      <c r="C46" s="441">
+        <v>710</v>
+      </c>
+      <c r="B46" s="447" t="s">
+        <v>711</v>
+      </c>
+      <c r="C46" s="442">
         <v>2.96</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>703</v>
+        <v>712</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>704</v>
+        <v>713</v>
       </c>
       <c r="F46" s="43">
         <v>80.0</v>
@@ -8321,38 +8356,38 @@
         <f t="shared" ref="L46:L78" si="8">I46*J46</f>
         <v>72.93</v>
       </c>
-      <c r="M46" s="439">
+      <c r="M46" s="440">
         <f t="shared" ref="M46:M78" si="9">I46/1000*$B$40^2</f>
         <v>1.287</v>
       </c>
-      <c r="N46" s="439">
+      <c r="N46" s="440">
         <f t="shared" ref="N46:N78" si="10">($B$39*$B$40*$B$41*1000*(J46*10^-9)/$B$42)*$B$43</f>
         <v>0.0363375</v>
       </c>
-      <c r="O46" s="439">
+      <c r="O46" s="440">
         <f t="shared" ref="O46:O78" si="11">K46*10^-9*$B$39*$B$41*1000</f>
         <v>0.0551</v>
       </c>
-      <c r="P46" s="439">
+      <c r="P46" s="440">
         <f t="shared" ref="P46:P78" si="12">M46+N46+O46</f>
         <v>1.3784375</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="3" t="s">
-        <v>705</v>
-      </c>
-      <c r="B47" s="446" t="s">
-        <v>706</v>
-      </c>
-      <c r="C47" s="441">
+        <v>714</v>
+      </c>
+      <c r="B47" s="447" t="s">
+        <v>715</v>
+      </c>
+      <c r="C47" s="442">
         <v>3.26</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>707</v>
+        <v>716</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>704</v>
+        <v>713</v>
       </c>
       <c r="F47" s="43">
         <v>60.0</v>
@@ -8376,19 +8411,19 @@
         <f t="shared" si="8"/>
         <v>139.5</v>
       </c>
-      <c r="M47" s="439">
+      <c r="M47" s="440">
         <f t="shared" si="9"/>
         <v>1.395</v>
       </c>
-      <c r="N47" s="439">
+      <c r="N47" s="440">
         <f t="shared" si="10"/>
         <v>0.064125</v>
       </c>
-      <c r="O47" s="439">
+      <c r="O47" s="440">
         <f t="shared" si="11"/>
         <v>0.00798</v>
       </c>
-      <c r="P47" s="439">
+      <c r="P47" s="440">
         <f t="shared" si="12"/>
         <v>1.467105</v>
       </c>
@@ -8397,17 +8432,17 @@
       <c r="A48" s="7" t="s">
         <v>439</v>
       </c>
-      <c r="B48" s="446" t="s">
-        <v>708</v>
-      </c>
-      <c r="C48" s="441">
+      <c r="B48" s="447" t="s">
+        <v>717</v>
+      </c>
+      <c r="C48" s="442">
         <v>2.63</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>707</v>
+        <v>716</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>704</v>
+        <v>713</v>
       </c>
       <c r="F48" s="43">
         <v>60.0</v>
@@ -8431,38 +8466,38 @@
         <f t="shared" si="8"/>
         <v>69</v>
       </c>
-      <c r="M48" s="439">
+      <c r="M48" s="440">
         <f t="shared" si="9"/>
         <v>2.07</v>
       </c>
-      <c r="N48" s="439">
+      <c r="N48" s="440">
         <f t="shared" si="10"/>
         <v>0.021375</v>
       </c>
-      <c r="O48" s="439">
+      <c r="O48" s="440">
         <f t="shared" si="11"/>
         <v>0.00684</v>
       </c>
-      <c r="P48" s="439">
+      <c r="P48" s="440">
         <f t="shared" si="12"/>
         <v>2.098215</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="7" t="s">
-        <v>709</v>
-      </c>
-      <c r="B49" s="446" t="s">
-        <v>710</v>
-      </c>
-      <c r="C49" s="441">
+        <v>718</v>
+      </c>
+      <c r="B49" s="447" t="s">
+        <v>719</v>
+      </c>
+      <c r="C49" s="442">
         <v>3.42</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>711</v>
+        <v>720</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>712</v>
+        <v>721</v>
       </c>
       <c r="F49" s="43">
         <v>100.0</v>
@@ -8486,38 +8521,38 @@
         <f t="shared" si="8"/>
         <v>22.08</v>
       </c>
-      <c r="M49" s="439">
+      <c r="M49" s="440">
         <f t="shared" si="9"/>
         <v>2.16</v>
       </c>
-      <c r="N49" s="439">
+      <c r="N49" s="440">
         <f t="shared" si="10"/>
         <v>0.006555</v>
       </c>
-      <c r="O49" s="439">
+      <c r="O49" s="440">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="P49" s="439">
+      <c r="P49" s="440">
         <f t="shared" si="12"/>
         <v>2.166555</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="3" t="s">
+        <v>722</v>
+      </c>
+      <c r="B50" s="447" t="s">
+        <v>723</v>
+      </c>
+      <c r="C50" s="442">
+        <v>1.46</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>724</v>
+      </c>
+      <c r="E50" s="3" t="s">
         <v>713</v>
-      </c>
-      <c r="B50" s="446" t="s">
-        <v>714</v>
-      </c>
-      <c r="C50" s="441">
-        <v>1.46</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>715</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>704</v>
       </c>
       <c r="F50" s="43">
         <v>60.0</v>
@@ -8541,38 +8576,38 @@
         <f t="shared" si="8"/>
         <v>124.8</v>
       </c>
-      <c r="M50" s="439">
+      <c r="M50" s="440">
         <f t="shared" si="9"/>
         <v>2.16</v>
       </c>
-      <c r="N50" s="439">
+      <c r="N50" s="440">
         <f t="shared" si="10"/>
         <v>0.03705</v>
       </c>
-      <c r="O50" s="439">
+      <c r="O50" s="440">
         <f t="shared" si="11"/>
         <v>0.0114</v>
       </c>
-      <c r="P50" s="439">
+      <c r="P50" s="440">
         <f t="shared" si="12"/>
         <v>2.20845</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="3" t="s">
-        <v>716</v>
-      </c>
-      <c r="B51" s="446" t="s">
-        <v>717</v>
-      </c>
-      <c r="C51" s="441">
+        <v>725</v>
+      </c>
+      <c r="B51" s="447" t="s">
+        <v>726</v>
+      </c>
+      <c r="C51" s="442">
         <v>2.32</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>718</v>
+        <v>727</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>704</v>
+        <v>713</v>
       </c>
       <c r="F51" s="43">
         <v>60.0</v>
@@ -8596,38 +8631,38 @@
         <f t="shared" si="8"/>
         <v>100</v>
       </c>
-      <c r="M51" s="439">
+      <c r="M51" s="440">
         <f t="shared" si="9"/>
         <v>2.25</v>
       </c>
-      <c r="N51" s="439">
+      <c r="N51" s="440">
         <f t="shared" si="10"/>
         <v>0.0285</v>
       </c>
-      <c r="O51" s="439">
+      <c r="O51" s="440">
         <f t="shared" si="11"/>
         <v>0.007258</v>
       </c>
-      <c r="P51" s="439">
+      <c r="P51" s="440">
         <f t="shared" si="12"/>
         <v>2.285758</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="3" t="s">
-        <v>719</v>
-      </c>
-      <c r="B52" s="437" t="s">
-        <v>720</v>
-      </c>
-      <c r="C52" s="441">
+        <v>728</v>
+      </c>
+      <c r="B52" s="438" t="s">
+        <v>729</v>
+      </c>
+      <c r="C52" s="442">
         <v>1.3</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>721</v>
+        <v>730</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>704</v>
+        <v>713</v>
       </c>
       <c r="F52" s="43">
         <v>60.0</v>
@@ -8651,38 +8686,38 @@
         <f t="shared" si="8"/>
         <v>177.5</v>
       </c>
-      <c r="M52" s="439">
+      <c r="M52" s="440">
         <f t="shared" si="9"/>
         <v>2.25</v>
       </c>
-      <c r="N52" s="439">
+      <c r="N52" s="440">
         <f t="shared" si="10"/>
         <v>0.0505875</v>
       </c>
-      <c r="O52" s="439">
+      <c r="O52" s="440">
         <f t="shared" si="11"/>
         <v>0.00969</v>
       </c>
-      <c r="P52" s="439">
+      <c r="P52" s="440">
         <f t="shared" si="12"/>
         <v>2.3102775</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="3" t="s">
-        <v>722</v>
-      </c>
-      <c r="B53" s="446" t="s">
-        <v>723</v>
-      </c>
-      <c r="C53" s="441">
+        <v>731</v>
+      </c>
+      <c r="B53" s="447" t="s">
+        <v>732</v>
+      </c>
+      <c r="C53" s="442">
         <v>3.93</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>707</v>
+        <v>716</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>704</v>
+        <v>713</v>
       </c>
       <c r="F53" s="43">
         <v>80.0</v>
@@ -8706,38 +8741,38 @@
         <f t="shared" si="8"/>
         <v>86.7</v>
       </c>
-      <c r="M53" s="439">
+      <c r="M53" s="440">
         <f t="shared" si="9"/>
         <v>2.295</v>
       </c>
-      <c r="N53" s="439">
+      <c r="N53" s="440">
         <f t="shared" si="10"/>
         <v>0.024225</v>
       </c>
-      <c r="O53" s="439">
+      <c r="O53" s="440">
         <f t="shared" si="11"/>
         <v>0.01083</v>
       </c>
-      <c r="P53" s="439">
+      <c r="P53" s="440">
         <f t="shared" si="12"/>
         <v>2.330055</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="3" t="s">
-        <v>724</v>
-      </c>
-      <c r="B54" s="447" t="s">
-        <v>725</v>
-      </c>
-      <c r="C54" s="441">
+        <v>733</v>
+      </c>
+      <c r="B54" s="448" t="s">
+        <v>734</v>
+      </c>
+      <c r="C54" s="442">
         <v>1.62</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>726</v>
+        <v>735</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>704</v>
+        <v>713</v>
       </c>
       <c r="F54" s="43">
         <v>80.0</v>
@@ -8761,38 +8796,38 @@
         <f t="shared" si="8"/>
         <v>72.8</v>
       </c>
-      <c r="M54" s="439">
+      <c r="M54" s="440">
         <f t="shared" si="9"/>
         <v>2.34</v>
       </c>
-      <c r="N54" s="439">
+      <c r="N54" s="440">
         <f t="shared" si="10"/>
         <v>0.01995</v>
       </c>
-      <c r="O54" s="439">
+      <c r="O54" s="440">
         <f t="shared" si="11"/>
         <v>0.03097</v>
       </c>
-      <c r="P54" s="439">
+      <c r="P54" s="440">
         <f t="shared" si="12"/>
         <v>2.39092</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="3" t="s">
-        <v>727</v>
-      </c>
-      <c r="B55" s="446" t="s">
-        <v>728</v>
-      </c>
-      <c r="C55" s="441">
+        <v>736</v>
+      </c>
+      <c r="B55" s="447" t="s">
+        <v>737</v>
+      </c>
+      <c r="C55" s="442">
         <v>1.62</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>707</v>
+        <v>716</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>704</v>
+        <v>713</v>
       </c>
       <c r="F55" s="43">
         <v>60.0</v>
@@ -8816,38 +8851,38 @@
         <f t="shared" si="8"/>
         <v>81</v>
       </c>
-      <c r="M55" s="439">
+      <c r="M55" s="440">
         <f t="shared" si="9"/>
         <v>2.43</v>
       </c>
-      <c r="N55" s="439">
+      <c r="N55" s="440">
         <f t="shared" si="10"/>
         <v>0.021375</v>
       </c>
-      <c r="O55" s="439">
+      <c r="O55" s="440">
         <f t="shared" si="11"/>
         <v>0.00684</v>
       </c>
-      <c r="P55" s="439">
+      <c r="P55" s="440">
         <f t="shared" si="12"/>
         <v>2.458215</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="3" t="s">
-        <v>729</v>
-      </c>
-      <c r="B56" s="447" t="s">
-        <v>730</v>
-      </c>
-      <c r="C56" s="441">
+        <v>738</v>
+      </c>
+      <c r="B56" s="448" t="s">
+        <v>739</v>
+      </c>
+      <c r="C56" s="442">
         <v>1.5</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>731</v>
+        <v>740</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>704</v>
+        <v>713</v>
       </c>
       <c r="F56" s="43">
         <v>60.0</v>
@@ -8871,38 +8906,38 @@
         <f t="shared" si="8"/>
         <v>58.8</v>
       </c>
-      <c r="M56" s="439">
+      <c r="M56" s="440">
         <f t="shared" si="9"/>
         <v>2.52</v>
       </c>
-      <c r="N56" s="439">
+      <c r="N56" s="440">
         <f t="shared" si="10"/>
         <v>0.0149625</v>
       </c>
-      <c r="O56" s="439">
+      <c r="O56" s="440">
         <f t="shared" si="11"/>
         <v>0.00931</v>
       </c>
-      <c r="P56" s="439">
+      <c r="P56" s="440">
         <f t="shared" si="12"/>
         <v>2.5442725</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="3" t="s">
-        <v>732</v>
-      </c>
-      <c r="B57" s="446" t="s">
-        <v>733</v>
-      </c>
-      <c r="C57" s="441">
+        <v>741</v>
+      </c>
+      <c r="B57" s="447" t="s">
+        <v>742</v>
+      </c>
+      <c r="C57" s="442">
         <v>2.26</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>707</v>
+        <v>716</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>704</v>
+        <v>713</v>
       </c>
       <c r="F57" s="43">
         <v>60.0</v>
@@ -8926,38 +8961,38 @@
         <f t="shared" si="8"/>
         <v>103.6</v>
       </c>
-      <c r="M57" s="439">
+      <c r="M57" s="440">
         <f t="shared" si="9"/>
         <v>2.52</v>
       </c>
-      <c r="N57" s="439">
+      <c r="N57" s="440">
         <f t="shared" si="10"/>
         <v>0.0263625</v>
       </c>
-      <c r="O57" s="439">
+      <c r="O57" s="440">
         <f t="shared" si="11"/>
         <v>0.00551</v>
       </c>
-      <c r="P57" s="439">
+      <c r="P57" s="440">
         <f t="shared" si="12"/>
         <v>2.5518725</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="3" t="s">
-        <v>734</v>
-      </c>
-      <c r="B58" s="437" t="s">
-        <v>735</v>
-      </c>
-      <c r="C58" s="441">
+        <v>743</v>
+      </c>
+      <c r="B58" s="438" t="s">
+        <v>744</v>
+      </c>
+      <c r="C58" s="442">
         <v>1.41</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>736</v>
+        <v>745</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>704</v>
+        <v>713</v>
       </c>
       <c r="F58" s="43">
         <v>60.0</v>
@@ -8981,38 +9016,38 @@
         <f t="shared" si="8"/>
         <v>168</v>
       </c>
-      <c r="M58" s="439">
+      <c r="M58" s="440">
         <f t="shared" si="9"/>
         <v>2.7</v>
       </c>
-      <c r="N58" s="439">
+      <c r="N58" s="440">
         <f t="shared" si="10"/>
         <v>0.0399</v>
       </c>
-      <c r="O58" s="439">
+      <c r="O58" s="440">
         <f t="shared" si="11"/>
         <v>0.01216</v>
       </c>
-      <c r="P58" s="439">
+      <c r="P58" s="440">
         <f t="shared" si="12"/>
         <v>2.75206</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="3" t="s">
-        <v>737</v>
-      </c>
-      <c r="B59" s="446" t="s">
-        <v>738</v>
-      </c>
-      <c r="C59" s="441">
+        <v>746</v>
+      </c>
+      <c r="B59" s="447" t="s">
+        <v>747</v>
+      </c>
+      <c r="C59" s="442">
         <v>1.93</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>739</v>
+        <v>748</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>704</v>
+        <v>713</v>
       </c>
       <c r="F59" s="43">
         <v>80.0</v>
@@ -9036,38 +9071,38 @@
         <f t="shared" si="8"/>
         <v>114</v>
       </c>
-      <c r="M59" s="439">
+      <c r="M59" s="440">
         <f t="shared" si="9"/>
         <v>2.7</v>
       </c>
-      <c r="N59" s="439">
+      <c r="N59" s="440">
         <f t="shared" si="10"/>
         <v>0.027075</v>
       </c>
-      <c r="O59" s="439">
+      <c r="O59" s="440">
         <f t="shared" si="11"/>
         <v>0.0285</v>
       </c>
-      <c r="P59" s="439">
+      <c r="P59" s="440">
         <f t="shared" si="12"/>
         <v>2.755575</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="3" t="s">
-        <v>740</v>
-      </c>
-      <c r="B60" s="446" t="s">
-        <v>741</v>
-      </c>
-      <c r="C60" s="441">
+        <v>749</v>
+      </c>
+      <c r="B60" s="447" t="s">
+        <v>750</v>
+      </c>
+      <c r="C60" s="442">
         <v>1.16</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>742</v>
+        <v>751</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>704</v>
+        <v>713</v>
       </c>
       <c r="F60" s="43">
         <v>80.0</v>
@@ -9091,38 +9126,38 @@
         <f t="shared" si="8"/>
         <v>55.8</v>
       </c>
-      <c r="M60" s="439">
+      <c r="M60" s="440">
         <f t="shared" si="9"/>
         <v>2.79</v>
       </c>
-      <c r="N60" s="439">
+      <c r="N60" s="440">
         <f t="shared" si="10"/>
         <v>0.012825</v>
       </c>
-      <c r="O60" s="439">
+      <c r="O60" s="440">
         <f t="shared" si="11"/>
         <v>0.01064</v>
       </c>
-      <c r="P60" s="439">
+      <c r="P60" s="440">
         <f t="shared" si="12"/>
         <v>2.813465</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="3" t="s">
-        <v>743</v>
-      </c>
-      <c r="B61" s="446" t="s">
-        <v>744</v>
-      </c>
-      <c r="C61" s="441">
+        <v>752</v>
+      </c>
+      <c r="B61" s="447" t="s">
+        <v>753</v>
+      </c>
+      <c r="C61" s="442">
         <v>7.15</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>745</v>
+        <v>754</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>712</v>
+        <v>721</v>
       </c>
       <c r="F61" s="43">
         <v>150.0</v>
@@ -9146,38 +9181,38 @@
         <f t="shared" si="8"/>
         <v>64</v>
       </c>
-      <c r="M61" s="439">
+      <c r="M61" s="440">
         <f t="shared" si="9"/>
         <v>2.88</v>
       </c>
-      <c r="N61" s="439">
+      <c r="N61" s="440">
         <f t="shared" si="10"/>
         <v>0.01425</v>
       </c>
-      <c r="O61" s="439">
+      <c r="O61" s="440">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="P61" s="439">
+      <c r="P61" s="440">
         <f t="shared" si="12"/>
         <v>2.89425</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="3" t="s">
-        <v>746</v>
-      </c>
-      <c r="B62" s="446" t="s">
-        <v>747</v>
-      </c>
-      <c r="C62" s="441">
+        <v>755</v>
+      </c>
+      <c r="B62" s="447" t="s">
+        <v>756</v>
+      </c>
+      <c r="C62" s="442">
         <v>1.64</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>748</v>
+        <v>757</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>704</v>
+        <v>713</v>
       </c>
       <c r="F62" s="43">
         <v>60.0</v>
@@ -9201,38 +9236,38 @@
         <f t="shared" si="8"/>
         <v>126.72</v>
       </c>
-      <c r="M62" s="439">
+      <c r="M62" s="440">
         <f t="shared" si="9"/>
         <v>2.88</v>
       </c>
-      <c r="N62" s="439">
+      <c r="N62" s="440">
         <f t="shared" si="10"/>
         <v>0.028215</v>
       </c>
-      <c r="O62" s="439">
+      <c r="O62" s="440">
         <f t="shared" si="11"/>
         <v>0.00722</v>
       </c>
-      <c r="P62" s="439">
+      <c r="P62" s="440">
         <f t="shared" si="12"/>
         <v>2.915435</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="3" t="s">
-        <v>749</v>
-      </c>
-      <c r="B63" s="437" t="s">
-        <v>750</v>
-      </c>
-      <c r="C63" s="441">
+        <v>758</v>
+      </c>
+      <c r="B63" s="438" t="s">
+        <v>759</v>
+      </c>
+      <c r="C63" s="442">
         <v>1.09</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>715</v>
+        <v>724</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>704</v>
+        <v>713</v>
       </c>
       <c r="F63" s="43">
         <v>60.0</v>
@@ -9256,38 +9291,38 @@
         <f t="shared" si="8"/>
         <v>112.2</v>
       </c>
-      <c r="M63" s="439">
+      <c r="M63" s="440">
         <f t="shared" si="9"/>
         <v>2.97</v>
       </c>
-      <c r="N63" s="439">
+      <c r="N63" s="440">
         <f t="shared" si="10"/>
         <v>0.024225</v>
       </c>
-      <c r="O63" s="439">
+      <c r="O63" s="440">
         <f t="shared" si="11"/>
         <v>0.00608</v>
       </c>
-      <c r="P63" s="439">
+      <c r="P63" s="440">
         <f t="shared" si="12"/>
         <v>3.000305</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="3" t="s">
-        <v>751</v>
-      </c>
-      <c r="B64" s="446" t="s">
-        <v>752</v>
-      </c>
-      <c r="C64" s="441">
+        <v>760</v>
+      </c>
+      <c r="B64" s="447" t="s">
+        <v>761</v>
+      </c>
+      <c r="C64" s="442">
         <v>1.2</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>707</v>
+        <v>716</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>704</v>
+        <v>713</v>
       </c>
       <c r="F64" s="43">
         <v>60.0</v>
@@ -9311,38 +9346,38 @@
         <f t="shared" si="8"/>
         <v>112.2</v>
       </c>
-      <c r="M64" s="439">
+      <c r="M64" s="440">
         <f t="shared" si="9"/>
         <v>3.06</v>
       </c>
-      <c r="N64" s="439">
+      <c r="N64" s="440">
         <f t="shared" si="10"/>
         <v>0.0235125</v>
       </c>
-      <c r="O64" s="439">
+      <c r="O64" s="440">
         <f t="shared" si="11"/>
         <v>0.01235</v>
       </c>
-      <c r="P64" s="439">
+      <c r="P64" s="440">
         <f t="shared" si="12"/>
         <v>3.0958625</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="3" t="s">
-        <v>753</v>
-      </c>
-      <c r="B65" s="446" t="s">
-        <v>754</v>
-      </c>
-      <c r="C65" s="441">
+        <v>762</v>
+      </c>
+      <c r="B65" s="447" t="s">
+        <v>763</v>
+      </c>
+      <c r="C65" s="442">
         <v>2.59</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>707</v>
+        <v>716</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>704</v>
+        <v>713</v>
       </c>
       <c r="F65" s="43">
         <v>100.0</v>
@@ -9366,38 +9401,38 @@
         <f t="shared" si="8"/>
         <v>156.4</v>
       </c>
-      <c r="M65" s="439">
+      <c r="M65" s="440">
         <f t="shared" si="9"/>
         <v>3.06</v>
       </c>
-      <c r="N65" s="439">
+      <c r="N65" s="440">
         <f t="shared" si="10"/>
         <v>0.032775</v>
       </c>
-      <c r="O65" s="439">
+      <c r="O65" s="440">
         <f t="shared" si="11"/>
         <v>0.00798</v>
       </c>
-      <c r="P65" s="439">
+      <c r="P65" s="440">
         <f t="shared" si="12"/>
         <v>3.100755</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="7" t="s">
-        <v>755</v>
-      </c>
-      <c r="B66" s="447" t="s">
-        <v>756</v>
-      </c>
-      <c r="C66" s="441">
+        <v>764</v>
+      </c>
+      <c r="B66" s="448" t="s">
+        <v>765</v>
+      </c>
+      <c r="C66" s="442">
         <v>3.94</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>757</v>
+        <v>766</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>704</v>
+        <v>713</v>
       </c>
       <c r="F66" s="43">
         <v>100.0</v>
@@ -9421,38 +9456,38 @@
         <f t="shared" si="8"/>
         <v>255</v>
       </c>
-      <c r="M66" s="439">
+      <c r="M66" s="440">
         <f t="shared" si="9"/>
         <v>3.06</v>
       </c>
-      <c r="N66" s="439">
+      <c r="N66" s="440">
         <f t="shared" si="10"/>
         <v>0.0534375</v>
       </c>
-      <c r="O66" s="439">
+      <c r="O66" s="440">
         <f t="shared" si="11"/>
         <v>0.08284</v>
       </c>
-      <c r="P66" s="439">
+      <c r="P66" s="440">
         <f t="shared" si="12"/>
         <v>3.1962775</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="3" t="s">
-        <v>758</v>
-      </c>
-      <c r="B67" s="446" t="s">
-        <v>759</v>
-      </c>
-      <c r="C67" s="441">
+        <v>767</v>
+      </c>
+      <c r="B67" s="447" t="s">
+        <v>768</v>
+      </c>
+      <c r="C67" s="442">
         <v>2.96</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>715</v>
+        <v>724</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>704</v>
+        <v>713</v>
       </c>
       <c r="F67" s="43">
         <v>100.0</v>
@@ -9476,38 +9511,38 @@
         <f t="shared" si="8"/>
         <v>104.4</v>
       </c>
-      <c r="M67" s="439">
+      <c r="M67" s="440">
         <f t="shared" si="9"/>
         <v>3.24</v>
       </c>
-      <c r="N67" s="439">
+      <c r="N67" s="440">
         <f t="shared" si="10"/>
         <v>0.0206625</v>
       </c>
-      <c r="O67" s="439">
+      <c r="O67" s="440">
         <f t="shared" si="11"/>
         <v>0.03477</v>
       </c>
-      <c r="P67" s="439">
+      <c r="P67" s="440">
         <f t="shared" si="12"/>
         <v>3.2954325</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="3" t="s">
-        <v>760</v>
-      </c>
-      <c r="B68" s="437" t="s">
-        <v>761</v>
-      </c>
-      <c r="C68" s="441">
+        <v>769</v>
+      </c>
+      <c r="B68" s="438" t="s">
+        <v>770</v>
+      </c>
+      <c r="C68" s="442">
         <v>1.59</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>762</v>
+        <v>771</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>704</v>
+        <v>713</v>
       </c>
       <c r="F68" s="43">
         <v>60.0</v>
@@ -9531,38 +9566,38 @@
         <f t="shared" si="8"/>
         <v>165.6</v>
       </c>
-      <c r="M68" s="439">
+      <c r="M68" s="440">
         <f t="shared" si="9"/>
         <v>4.14</v>
       </c>
-      <c r="N68" s="439">
+      <c r="N68" s="440">
         <f t="shared" si="10"/>
         <v>0.02565</v>
       </c>
-      <c r="O68" s="439">
+      <c r="O68" s="440">
         <f t="shared" si="11"/>
         <v>0.019</v>
       </c>
-      <c r="P68" s="439">
+      <c r="P68" s="440">
         <f t="shared" si="12"/>
         <v>4.18465</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="3" t="s">
-        <v>763</v>
-      </c>
-      <c r="B69" s="437" t="s">
-        <v>764</v>
-      </c>
-      <c r="C69" s="441">
+        <v>772</v>
+      </c>
+      <c r="B69" s="438" t="s">
+        <v>773</v>
+      </c>
+      <c r="C69" s="442">
         <v>0.772</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>765</v>
+        <v>774</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>704</v>
+        <v>713</v>
       </c>
       <c r="F69" s="43">
         <v>60.0</v>
@@ -9586,38 +9621,38 @@
         <f t="shared" si="8"/>
         <v>412.8</v>
       </c>
-      <c r="M69" s="439">
+      <c r="M69" s="440">
         <f t="shared" si="9"/>
         <v>4.32</v>
       </c>
-      <c r="N69" s="439">
+      <c r="N69" s="440">
         <f t="shared" si="10"/>
         <v>0.061275</v>
       </c>
-      <c r="O69" s="439">
+      <c r="O69" s="440">
         <f t="shared" si="11"/>
         <v>0.00684</v>
       </c>
-      <c r="P69" s="439">
+      <c r="P69" s="440">
         <f t="shared" si="12"/>
         <v>4.388115</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="3" t="s">
-        <v>766</v>
-      </c>
-      <c r="B70" s="440" t="s">
-        <v>767</v>
-      </c>
-      <c r="C70" s="441">
+        <v>775</v>
+      </c>
+      <c r="B70" s="441" t="s">
+        <v>776</v>
+      </c>
+      <c r="C70" s="442">
         <v>1.97</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>762</v>
+        <v>771</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>704</v>
+        <v>713</v>
       </c>
       <c r="F70" s="43">
         <v>100.0</v>
@@ -9641,38 +9676,38 @@
         <f t="shared" si="8"/>
         <v>196.1</v>
       </c>
-      <c r="M70" s="439">
+      <c r="M70" s="440">
         <f t="shared" si="9"/>
         <v>4.77</v>
       </c>
-      <c r="N70" s="439">
+      <c r="N70" s="440">
         <f t="shared" si="10"/>
         <v>0.0263625</v>
       </c>
-      <c r="O70" s="439">
+      <c r="O70" s="440">
         <f t="shared" si="11"/>
         <v>0.04294</v>
       </c>
-      <c r="P70" s="439">
+      <c r="P70" s="440">
         <f t="shared" si="12"/>
         <v>4.8393025</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="3" t="s">
-        <v>768</v>
-      </c>
-      <c r="B71" s="437" t="s">
-        <v>769</v>
-      </c>
-      <c r="C71" s="441">
+        <v>777</v>
+      </c>
+      <c r="B71" s="438" t="s">
+        <v>778</v>
+      </c>
+      <c r="C71" s="442">
         <v>0.725</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>770</v>
+        <v>779</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>704</v>
+        <v>713</v>
       </c>
       <c r="F71" s="43">
         <v>60.0</v>
@@ -9696,38 +9731,38 @@
         <f t="shared" si="8"/>
         <v>118.8</v>
       </c>
-      <c r="M71" s="439">
+      <c r="M71" s="440">
         <f t="shared" si="9"/>
         <v>4.86</v>
       </c>
-      <c r="N71" s="439">
+      <c r="N71" s="440">
         <f t="shared" si="10"/>
         <v>0.015675</v>
       </c>
-      <c r="O71" s="439">
+      <c r="O71" s="440">
         <f t="shared" si="11"/>
         <v>0.00532</v>
       </c>
-      <c r="P71" s="439">
+      <c r="P71" s="440">
         <f t="shared" si="12"/>
         <v>4.880995</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="3" t="s">
-        <v>771</v>
-      </c>
-      <c r="B72" s="446" t="s">
-        <v>772</v>
-      </c>
-      <c r="C72" s="441">
+        <v>780</v>
+      </c>
+      <c r="B72" s="447" t="s">
+        <v>781</v>
+      </c>
+      <c r="C72" s="442">
         <v>5.05</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>773</v>
+        <v>782</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>712</v>
+        <v>721</v>
       </c>
       <c r="F72" s="43">
         <v>100.0</v>
@@ -9751,38 +9786,38 @@
         <f t="shared" si="8"/>
         <v>50.6</v>
       </c>
-      <c r="M72" s="439">
+      <c r="M72" s="440">
         <f t="shared" si="9"/>
         <v>4.95</v>
       </c>
-      <c r="N72" s="439">
+      <c r="N72" s="440">
         <f t="shared" si="10"/>
         <v>0.006555</v>
       </c>
-      <c r="O72" s="439">
+      <c r="O72" s="440">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="P72" s="439">
+      <c r="P72" s="440">
         <f t="shared" si="12"/>
         <v>4.956555</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="7" t="s">
-        <v>774</v>
-      </c>
-      <c r="B73" s="447" t="s">
-        <v>775</v>
-      </c>
-      <c r="C73" s="441">
+        <v>783</v>
+      </c>
+      <c r="B73" s="448" t="s">
+        <v>784</v>
+      </c>
+      <c r="C73" s="442">
         <v>2.73</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>776</v>
+        <v>785</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>712</v>
+        <v>721</v>
       </c>
       <c r="F73" s="43">
         <v>150.0</v>
@@ -9806,38 +9841,38 @@
         <f t="shared" si="8"/>
         <v>42.56</v>
       </c>
-      <c r="M73" s="439">
+      <c r="M73" s="440">
         <f t="shared" si="9"/>
         <v>5.04</v>
       </c>
-      <c r="N73" s="439">
+      <c r="N73" s="440">
         <f t="shared" si="10"/>
         <v>0.005415</v>
       </c>
-      <c r="O73" s="439">
+      <c r="O73" s="440">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="P73" s="439">
+      <c r="P73" s="440">
         <f t="shared" si="12"/>
         <v>5.045415</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="7" t="s">
-        <v>777</v>
-      </c>
-      <c r="B74" s="446" t="s">
-        <v>778</v>
-      </c>
-      <c r="C74" s="441">
+        <v>786</v>
+      </c>
+      <c r="B74" s="447" t="s">
+        <v>787</v>
+      </c>
+      <c r="C74" s="442">
         <v>2.19</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>757</v>
+        <v>766</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>704</v>
+        <v>713</v>
       </c>
       <c r="F74" s="43">
         <v>100.0</v>
@@ -9861,38 +9896,38 @@
         <f t="shared" si="8"/>
         <v>246.4</v>
       </c>
-      <c r="M74" s="439">
+      <c r="M74" s="440">
         <f t="shared" si="9"/>
         <v>5.04</v>
       </c>
-      <c r="N74" s="439">
+      <c r="N74" s="440">
         <f t="shared" si="10"/>
         <v>0.03135</v>
       </c>
-      <c r="O74" s="439">
+      <c r="O74" s="440">
         <f t="shared" si="11"/>
         <v>0.06194</v>
       </c>
-      <c r="P74" s="439">
+      <c r="P74" s="440">
         <f t="shared" si="12"/>
         <v>5.13329</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="3" t="s">
-        <v>779</v>
-      </c>
-      <c r="B75" s="446" t="s">
-        <v>780</v>
-      </c>
-      <c r="C75" s="441">
+        <v>788</v>
+      </c>
+      <c r="B75" s="447" t="s">
+        <v>789</v>
+      </c>
+      <c r="C75" s="442">
         <v>8.3</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>781</v>
+        <v>790</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>712</v>
+        <v>721</v>
       </c>
       <c r="F75" s="43">
         <v>100.0</v>
@@ -9916,38 +9951,38 @@
         <f t="shared" si="8"/>
         <v>56</v>
       </c>
-      <c r="M75" s="439">
+      <c r="M75" s="440">
         <f t="shared" si="9"/>
         <v>6.3</v>
       </c>
-      <c r="N75" s="439">
+      <c r="N75" s="440">
         <f t="shared" si="10"/>
         <v>0.0057</v>
       </c>
-      <c r="O75" s="439">
+      <c r="O75" s="440">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="P75" s="439">
+      <c r="P75" s="440">
         <f t="shared" si="12"/>
         <v>6.3057</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="7" t="s">
-        <v>782</v>
-      </c>
-      <c r="B76" s="446" t="s">
-        <v>783</v>
-      </c>
-      <c r="C76" s="441">
+        <v>791</v>
+      </c>
+      <c r="B76" s="447" t="s">
+        <v>792</v>
+      </c>
+      <c r="C76" s="442">
         <v>3.26</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>757</v>
+        <v>766</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>704</v>
+        <v>713</v>
       </c>
       <c r="F76" s="43">
         <v>150.0</v>
@@ -9971,38 +10006,38 @@
         <f t="shared" si="8"/>
         <v>386.9</v>
       </c>
-      <c r="M76" s="439">
+      <c r="M76" s="440">
         <f t="shared" si="9"/>
         <v>6.57</v>
       </c>
-      <c r="N76" s="439">
+      <c r="N76" s="440">
         <f t="shared" si="10"/>
         <v>0.0377625</v>
       </c>
-      <c r="O76" s="439">
+      <c r="O76" s="440">
         <f t="shared" si="11"/>
         <v>0.04693</v>
       </c>
-      <c r="P76" s="439">
+      <c r="P76" s="440">
         <f t="shared" si="12"/>
         <v>6.6546925</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="7" t="s">
-        <v>784</v>
-      </c>
-      <c r="B77" s="446" t="s">
-        <v>785</v>
-      </c>
-      <c r="C77" s="441">
+        <v>793</v>
+      </c>
+      <c r="B77" s="447" t="s">
+        <v>794</v>
+      </c>
+      <c r="C77" s="442">
         <v>1.84</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>757</v>
+        <v>766</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>704</v>
+        <v>713</v>
       </c>
       <c r="F77" s="43">
         <v>100.0</v>
@@ -10026,38 +10061,38 @@
         <f t="shared" si="8"/>
         <v>292.6</v>
       </c>
-      <c r="M77" s="439">
+      <c r="M77" s="440">
         <f t="shared" si="9"/>
         <v>6.93</v>
       </c>
-      <c r="N77" s="439">
+      <c r="N77" s="440">
         <f t="shared" si="10"/>
         <v>0.027075</v>
       </c>
-      <c r="O77" s="439">
+      <c r="O77" s="440">
         <f t="shared" si="11"/>
         <v>0.0513</v>
       </c>
-      <c r="P77" s="439">
+      <c r="P77" s="440">
         <f t="shared" si="12"/>
         <v>7.008375</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="3" t="s">
-        <v>786</v>
-      </c>
-      <c r="B78" s="446" t="s">
-        <v>787</v>
-      </c>
-      <c r="C78" s="441">
+        <v>795</v>
+      </c>
+      <c r="B78" s="447" t="s">
+        <v>796</v>
+      </c>
+      <c r="C78" s="442">
         <v>4.61</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>788</v>
+        <v>797</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>789</v>
+        <v>798</v>
       </c>
       <c r="F78" s="43">
         <v>100.0</v>
@@ -10081,28 +10116,28 @@
         <f t="shared" si="8"/>
         <v>52.8</v>
       </c>
-      <c r="M78" s="439">
+      <c r="M78" s="440">
         <f t="shared" si="9"/>
         <v>14.4</v>
       </c>
-      <c r="N78" s="439">
+      <c r="N78" s="440">
         <f t="shared" si="10"/>
         <v>0.00235125</v>
       </c>
-      <c r="O78" s="439">
+      <c r="O78" s="440">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="P78" s="439">
+      <c r="P78" s="440">
         <f t="shared" si="12"/>
         <v>14.40235125</v>
       </c>
     </row>
     <row r="79">
-      <c r="C79" s="448"/>
+      <c r="C79" s="449"/>
     </row>
     <row r="80">
-      <c r="C80" s="448"/>
+      <c r="C80" s="449"/>
     </row>
   </sheetData>
   <autoFilter ref="$A$7:$M$35">
@@ -74784,7 +74819,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="12.13"/>
+    <col customWidth="1" min="2" max="2" width="13.5"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -75354,6 +75389,88 @@
       </c>
       <c r="D24" s="426" t="s">
         <v>120</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" s="378" t="s">
+        <v>617</v>
+      </c>
+      <c r="C26" s="408"/>
+      <c r="D26" s="409"/>
+    </row>
+    <row r="27">
+      <c r="B27" s="415" t="s">
+        <v>618</v>
+      </c>
+      <c r="C27" s="395">
+        <v>92.2</v>
+      </c>
+      <c r="D27" s="414" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" s="415" t="s">
+        <v>619</v>
+      </c>
+      <c r="C28" s="395">
+        <v>1.0</v>
+      </c>
+      <c r="D28" s="414" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" s="415" t="s">
+        <v>620</v>
+      </c>
+      <c r="C29" s="395">
+        <v>1650.0</v>
+      </c>
+      <c r="D29" s="414"/>
+    </row>
+    <row r="30">
+      <c r="B30" s="415" t="s">
+        <v>621</v>
+      </c>
+      <c r="C30" s="395">
+        <v>125.0</v>
+      </c>
+      <c r="D30" s="414" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="B31" s="415" t="s">
+        <v>622</v>
+      </c>
+      <c r="C31" s="395">
+        <v>28.0</v>
+      </c>
+      <c r="D31" s="414"/>
+    </row>
+    <row r="32">
+      <c r="B32" s="415" t="s">
+        <v>623</v>
+      </c>
+      <c r="C32" s="394">
+        <f>C31^2/(C33*10^-6)</f>
+        <v>116.7000993</v>
+      </c>
+      <c r="D32" s="414" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" s="418" t="s">
+        <v>624</v>
+      </c>
+      <c r="C33" s="400">
+        <f>(((C27-C28)/1000)/(4*pi()*10^-7*C29*C30*10^-6))+((C28/1000)/(4*pi()*10^-7*1*C30*10^-6))</f>
+        <v>6718074.834</v>
+      </c>
+      <c r="D33" s="427" t="s">
+        <v>625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added transformer calc for LTspice
</commit_message>
<xml_diff>
--- a/documentation/DCDCv9-3_Table.xlsx
+++ b/documentation/DCDCv9-3_Table.xlsx
@@ -169,7 +169,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3287" uniqueCount="799">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3299" uniqueCount="808">
   <si>
     <t>DCDCv9-3 Table</t>
   </si>
@@ -2389,28 +2389,55 @@
     <t>UCC25600 dead time calc</t>
   </si>
   <si>
+    <t>Coupling factor calculator</t>
+  </si>
+  <si>
     <t>Resistance</t>
   </si>
   <si>
     <t>kΩ</t>
   </si>
   <si>
+    <t>Primary Inductance</t>
+  </si>
+  <si>
     <t>dead time</t>
   </si>
   <si>
+    <t>Primary leakage Ind.</t>
+  </si>
+  <si>
+    <t>Primary Windings</t>
+  </si>
+  <si>
     <t>Inductance calculator with air gap</t>
   </si>
   <si>
+    <t>Secondary Windings</t>
+  </si>
+  <si>
     <t>Mag. total length.</t>
   </si>
   <si>
+    <t>Winding Ratio</t>
+  </si>
+  <si>
     <t>Air gap length</t>
   </si>
   <si>
+    <t>Coupling factor (K)</t>
+  </si>
+  <si>
     <t>µ_r core</t>
   </si>
   <si>
+    <t>Secondary Inductance</t>
+  </si>
+  <si>
     <t>Cross-sectional area</t>
+  </si>
+  <si>
+    <t>Lp to Lr ratio  (M)</t>
   </si>
   <si>
     <t>Number of turns</t>
@@ -4214,7 +4241,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="450">
+  <cellXfs count="454">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -5464,6 +5491,9 @@
     <xf borderId="12" fillId="0" fontId="12" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="11" fillId="0" fontId="6" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="13" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
@@ -5475,6 +5505,13 @@
     </xf>
     <xf borderId="16" fillId="0" fontId="6" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="13" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="14" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="5" fontId="6" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="16" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
@@ -5754,11 +5791,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="22909543"/>
-        <c:axId val="277121533"/>
+        <c:axId val="1120502013"/>
+        <c:axId val="266073632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="22909543"/>
+        <c:axId val="1120502013"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5810,10 +5847,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="277121533"/>
+        <c:crossAx val="266073632"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="277121533"/>
+        <c:axId val="266073632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5888,7 +5925,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22909543"/>
+        <c:crossAx val="1120502013"/>
         <c:majorUnit val="0.2"/>
         <c:minorUnit val="0.1"/>
       </c:valAx>
@@ -5990,11 +6027,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="535757047"/>
-        <c:axId val="43241536"/>
+        <c:axId val="348862"/>
+        <c:axId val="1365550478"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="535757047"/>
+        <c:axId val="348862"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="52.0"/>
@@ -6047,10 +6084,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43241536"/>
+        <c:crossAx val="1365550478"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="43241536"/>
+        <c:axId val="1365550478"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6125,7 +6162,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="535757047"/>
+        <c:crossAx val="348862"/>
         <c:majorUnit val="0.2"/>
         <c:minorUnit val="0.1"/>
       </c:valAx>
@@ -6724,130 +6761,130 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="7" t="s">
-        <v>626</v>
+        <v>635</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="7"/>
-      <c r="E1" s="428"/>
+      <c r="E1" s="432"/>
     </row>
     <row r="2">
-      <c r="A2" s="429" t="s">
-        <v>627</v>
-      </c>
-      <c r="B2" s="430">
+      <c r="A2" s="433" t="s">
+        <v>636</v>
+      </c>
+      <c r="B2" s="434">
         <v>600.0</v>
       </c>
-      <c r="C2" s="431" t="s">
+      <c r="C2" s="435" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="432" t="s">
-        <v>628</v>
+      <c r="A3" s="436" t="s">
+        <v>637</v>
       </c>
       <c r="B3" s="18">
         <v>4.0</v>
       </c>
-      <c r="C3" s="433" t="s">
-        <v>629</v>
+      <c r="C3" s="437" t="s">
+        <v>638</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="432" t="s">
-        <v>630</v>
+      <c r="A4" s="436" t="s">
+        <v>639</v>
       </c>
       <c r="B4" s="3">
         <v>150.0</v>
       </c>
-      <c r="C4" s="433" t="s">
+      <c r="C4" s="437" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="432" t="s">
-        <v>631</v>
+      <c r="A5" s="436" t="s">
+        <v>640</v>
       </c>
       <c r="B5" s="18">
         <v>4.0</v>
       </c>
-      <c r="C5" s="433" t="s">
+      <c r="C5" s="437" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="434" t="s">
-        <v>632</v>
-      </c>
-      <c r="B6" s="435">
+      <c r="A6" s="438" t="s">
+        <v>641</v>
+      </c>
+      <c r="B6" s="439">
         <v>0.5</v>
       </c>
-      <c r="C6" s="436" t="s">
-        <v>633</v>
+      <c r="C6" s="440" t="s">
+        <v>642</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="40" t="s">
-        <v>634</v>
+        <v>643</v>
       </c>
       <c r="B7" s="40" t="s">
-        <v>635</v>
+        <v>644</v>
       </c>
       <c r="C7" s="40" t="s">
-        <v>636</v>
+        <v>645</v>
       </c>
       <c r="D7" s="40" t="s">
-        <v>637</v>
+        <v>646</v>
       </c>
       <c r="E7" s="40" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="F7" s="40" t="s">
-        <v>639</v>
+        <v>648</v>
       </c>
       <c r="G7" s="40" t="s">
-        <v>640</v>
+        <v>649</v>
       </c>
       <c r="H7" s="40" t="s">
-        <v>641</v>
+        <v>650</v>
       </c>
       <c r="I7" s="40" t="s">
-        <v>642</v>
+        <v>651</v>
       </c>
       <c r="J7" s="40" t="s">
-        <v>643</v>
+        <v>652</v>
       </c>
       <c r="K7" s="40" t="s">
-        <v>644</v>
+        <v>653</v>
       </c>
       <c r="L7" s="40" t="s">
-        <v>645</v>
+        <v>654</v>
       </c>
       <c r="M7" s="40" t="s">
-        <v>646</v>
-      </c>
-      <c r="N7" s="437"/>
-      <c r="O7" s="437"/>
-      <c r="P7" s="437"/>
-      <c r="Q7" s="437"/>
-      <c r="R7" s="437"/>
-      <c r="S7" s="437"/>
-      <c r="T7" s="437"/>
-      <c r="U7" s="437"/>
-      <c r="V7" s="437"/>
-      <c r="W7" s="437"/>
-      <c r="X7" s="437"/>
-      <c r="Y7" s="437"/>
-      <c r="Z7" s="437"/>
+        <v>655</v>
+      </c>
+      <c r="N7" s="441"/>
+      <c r="O7" s="441"/>
+      <c r="P7" s="441"/>
+      <c r="Q7" s="441"/>
+      <c r="R7" s="441"/>
+      <c r="S7" s="441"/>
+      <c r="T7" s="441"/>
+      <c r="U7" s="441"/>
+      <c r="V7" s="441"/>
+      <c r="W7" s="441"/>
+      <c r="X7" s="441"/>
+      <c r="Y7" s="441"/>
+      <c r="Z7" s="441"/>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>647</v>
-      </c>
-      <c r="B8" s="438" t="s">
-        <v>648</v>
-      </c>
-      <c r="C8" s="439">
+        <v>656</v>
+      </c>
+      <c r="B8" s="442" t="s">
+        <v>657</v>
+      </c>
+      <c r="C8" s="443">
         <v>41.11</v>
       </c>
       <c r="D8" s="43">
@@ -6863,19 +6900,19 @@
         <f t="shared" ref="G8:G35" si="1">D8*E8</f>
         <v>454.4</v>
       </c>
-      <c r="H8" s="440">
+      <c r="H8" s="444">
         <f t="shared" ref="H8:H35" si="2">D8/1000*$B$3^2</f>
         <v>0.512</v>
       </c>
-      <c r="I8" s="440">
+      <c r="I8" s="444">
         <f t="shared" ref="I8:I35" si="3">($B$2*$B$3*$B$4*1000*(E8*10^-9)/$B$5)*$B$6</f>
         <v>0.639</v>
       </c>
-      <c r="J8" s="440">
+      <c r="J8" s="444">
         <f t="shared" ref="J8:J35" si="4">F8*10^-9*$B$2*$B$4*1000</f>
         <v>0</v>
       </c>
-      <c r="K8" s="440">
+      <c r="K8" s="444">
         <f t="shared" ref="K8:K35" si="5">H8+I8+J8</f>
         <v>1.151</v>
       </c>
@@ -6890,12 +6927,12 @@
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>649</v>
-      </c>
-      <c r="B9" s="441" t="s">
-        <v>650</v>
-      </c>
-      <c r="C9" s="439">
+        <v>658</v>
+      </c>
+      <c r="B9" s="445" t="s">
+        <v>659</v>
+      </c>
+      <c r="C9" s="443">
         <v>13.32</v>
       </c>
       <c r="D9" s="43">
@@ -6911,19 +6948,19 @@
         <f t="shared" si="1"/>
         <v>406</v>
       </c>
-      <c r="H9" s="440">
+      <c r="H9" s="444">
         <f t="shared" si="2"/>
         <v>1.12</v>
       </c>
-      <c r="I9" s="440">
+      <c r="I9" s="444">
         <f t="shared" si="3"/>
         <v>0.261</v>
       </c>
-      <c r="J9" s="440">
+      <c r="J9" s="444">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K9" s="440">
+      <c r="K9" s="444">
         <f t="shared" si="5"/>
         <v>1.381</v>
       </c>
@@ -6938,12 +6975,12 @@
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>651</v>
-      </c>
-      <c r="B10" s="441" t="s">
-        <v>652</v>
-      </c>
-      <c r="C10" s="439">
+        <v>660</v>
+      </c>
+      <c r="B10" s="445" t="s">
+        <v>661</v>
+      </c>
+      <c r="C10" s="443">
         <v>12.8</v>
       </c>
       <c r="D10" s="43">
@@ -6959,19 +6996,19 @@
         <f t="shared" si="1"/>
         <v>429</v>
       </c>
-      <c r="H10" s="440">
+      <c r="H10" s="444">
         <f t="shared" si="2"/>
         <v>2.08</v>
       </c>
-      <c r="I10" s="440">
+      <c r="I10" s="444">
         <f t="shared" si="3"/>
         <v>0.1485</v>
       </c>
-      <c r="J10" s="440">
+      <c r="J10" s="444">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K10" s="440">
+      <c r="K10" s="444">
         <f t="shared" si="5"/>
         <v>2.2285</v>
       </c>
@@ -6986,12 +7023,12 @@
     </row>
     <row r="11">
       <c r="A11" s="7" t="s">
-        <v>653</v>
-      </c>
-      <c r="B11" s="438" t="s">
-        <v>654</v>
-      </c>
-      <c r="C11" s="439">
+        <v>662</v>
+      </c>
+      <c r="B11" s="442" t="s">
+        <v>663</v>
+      </c>
+      <c r="C11" s="443">
         <v>8.3</v>
       </c>
       <c r="D11" s="43">
@@ -7007,19 +7044,19 @@
         <f t="shared" si="1"/>
         <v>1364</v>
       </c>
-      <c r="H11" s="440">
+      <c r="H11" s="444">
         <f t="shared" si="2"/>
         <v>0.992</v>
       </c>
-      <c r="I11" s="440">
+      <c r="I11" s="444">
         <f t="shared" si="3"/>
         <v>0.99</v>
       </c>
-      <c r="J11" s="440">
+      <c r="J11" s="444">
         <f t="shared" si="4"/>
         <v>3.96</v>
       </c>
-      <c r="K11" s="440">
+      <c r="K11" s="444">
         <f t="shared" si="5"/>
         <v>5.942</v>
       </c>
@@ -7034,12 +7071,12 @@
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>655</v>
-      </c>
-      <c r="B12" s="438" t="s">
-        <v>656</v>
-      </c>
-      <c r="C12" s="439">
+        <v>664</v>
+      </c>
+      <c r="B12" s="442" t="s">
+        <v>665</v>
+      </c>
+      <c r="C12" s="443">
         <v>10.25</v>
       </c>
       <c r="D12" s="43">
@@ -7055,19 +7092,19 @@
         <f t="shared" si="1"/>
         <v>1372</v>
       </c>
-      <c r="H12" s="440">
+      <c r="H12" s="444">
         <f t="shared" si="2"/>
         <v>0.784</v>
       </c>
-      <c r="I12" s="440">
+      <c r="I12" s="444">
         <f t="shared" si="3"/>
         <v>1.26</v>
       </c>
-      <c r="J12" s="440">
+      <c r="J12" s="444">
         <f t="shared" si="4"/>
         <v>5.04</v>
       </c>
-      <c r="K12" s="440">
+      <c r="K12" s="444">
         <f t="shared" si="5"/>
         <v>7.084</v>
       </c>
@@ -7082,12 +7119,12 @@
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>657</v>
-      </c>
-      <c r="B13" s="441" t="s">
-        <v>658</v>
-      </c>
-      <c r="C13" s="439">
+        <v>666</v>
+      </c>
+      <c r="B13" s="445" t="s">
+        <v>667</v>
+      </c>
+      <c r="C13" s="443">
         <v>5.59</v>
       </c>
       <c r="D13" s="43">
@@ -7103,19 +7140,19 @@
         <f t="shared" si="1"/>
         <v>2184</v>
       </c>
-      <c r="H13" s="440">
+      <c r="H13" s="444">
         <f t="shared" si="2"/>
         <v>2.912</v>
       </c>
-      <c r="I13" s="440">
+      <c r="I13" s="444">
         <f t="shared" si="3"/>
         <v>0.54</v>
       </c>
-      <c r="J13" s="440">
+      <c r="J13" s="444">
         <f t="shared" si="4"/>
         <v>4.14</v>
       </c>
-      <c r="K13" s="440">
+      <c r="K13" s="444">
         <f t="shared" si="5"/>
         <v>7.592</v>
       </c>
@@ -7130,12 +7167,12 @@
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>659</v>
-      </c>
-      <c r="B14" s="438" t="s">
-        <v>660</v>
-      </c>
-      <c r="C14" s="439">
+        <v>668</v>
+      </c>
+      <c r="B14" s="442" t="s">
+        <v>669</v>
+      </c>
+      <c r="C14" s="443">
         <v>8.15</v>
       </c>
       <c r="D14" s="43">
@@ -7151,19 +7188,19 @@
         <f t="shared" si="1"/>
         <v>1955</v>
       </c>
-      <c r="H14" s="440">
+      <c r="H14" s="444">
         <f t="shared" si="2"/>
         <v>1.36</v>
       </c>
-      <c r="I14" s="440">
+      <c r="I14" s="444">
         <f t="shared" si="3"/>
         <v>1.035</v>
       </c>
-      <c r="J14" s="440">
+      <c r="J14" s="444">
         <f t="shared" si="4"/>
         <v>6.21</v>
       </c>
-      <c r="K14" s="440">
+      <c r="K14" s="444">
         <f t="shared" si="5"/>
         <v>8.605</v>
       </c>
@@ -7178,12 +7215,12 @@
     </row>
     <row r="15">
       <c r="A15" s="7" t="s">
-        <v>661</v>
-      </c>
-      <c r="B15" s="441" t="s">
-        <v>662</v>
-      </c>
-      <c r="C15" s="439">
+        <v>670</v>
+      </c>
+      <c r="B15" s="445" t="s">
+        <v>671</v>
+      </c>
+      <c r="C15" s="443">
         <v>7.38</v>
       </c>
       <c r="D15" s="43">
@@ -7199,19 +7236,19 @@
         <f t="shared" si="1"/>
         <v>2797.2</v>
       </c>
-      <c r="H15" s="440">
+      <c r="H15" s="444">
         <f t="shared" si="2"/>
         <v>1.184</v>
       </c>
-      <c r="I15" s="440">
+      <c r="I15" s="444">
         <f t="shared" si="3"/>
         <v>1.701</v>
       </c>
-      <c r="J15" s="440">
+      <c r="J15" s="444">
         <f t="shared" si="4"/>
         <v>6.93</v>
       </c>
-      <c r="K15" s="440">
+      <c r="K15" s="444">
         <f t="shared" si="5"/>
         <v>9.815</v>
       </c>
@@ -7226,12 +7263,12 @@
     </row>
     <row r="16">
       <c r="A16" s="7" t="s">
-        <v>663</v>
-      </c>
-      <c r="B16" s="441" t="s">
-        <v>664</v>
-      </c>
-      <c r="C16" s="439">
+        <v>672</v>
+      </c>
+      <c r="B16" s="445" t="s">
+        <v>673</v>
+      </c>
+      <c r="C16" s="443">
         <v>10.16</v>
       </c>
       <c r="D16" s="43">
@@ -7247,19 +7284,19 @@
         <f t="shared" si="1"/>
         <v>2112</v>
       </c>
-      <c r="H16" s="440">
+      <c r="H16" s="444">
         <f t="shared" si="2"/>
         <v>1.024</v>
       </c>
-      <c r="I16" s="440">
+      <c r="I16" s="444">
         <f t="shared" si="3"/>
         <v>1.485</v>
       </c>
-      <c r="J16" s="440">
+      <c r="J16" s="444">
         <f t="shared" si="4"/>
         <v>7.38</v>
       </c>
-      <c r="K16" s="440">
+      <c r="K16" s="444">
         <f t="shared" si="5"/>
         <v>9.889</v>
       </c>
@@ -7274,12 +7311,12 @@
     </row>
     <row r="17">
       <c r="A17" s="3" t="s">
-        <v>665</v>
-      </c>
-      <c r="B17" s="438" t="s">
-        <v>666</v>
-      </c>
-      <c r="C17" s="439">
+        <v>674</v>
+      </c>
+      <c r="B17" s="442" t="s">
+        <v>675</v>
+      </c>
+      <c r="C17" s="443">
         <v>9.95</v>
       </c>
       <c r="D17" s="43">
@@ -7295,19 +7332,19 @@
         <f t="shared" si="1"/>
         <v>1920</v>
       </c>
-      <c r="H17" s="440">
+      <c r="H17" s="444">
         <f t="shared" si="2"/>
         <v>1.28</v>
       </c>
-      <c r="I17" s="440">
+      <c r="I17" s="444">
         <f t="shared" si="3"/>
         <v>1.08</v>
       </c>
-      <c r="J17" s="440">
+      <c r="J17" s="444">
         <f t="shared" si="4"/>
         <v>7.65</v>
       </c>
-      <c r="K17" s="440">
+      <c r="K17" s="444">
         <f t="shared" si="5"/>
         <v>10.01</v>
       </c>
@@ -7322,12 +7359,12 @@
     </row>
     <row r="18">
       <c r="A18" s="3" t="s">
-        <v>667</v>
-      </c>
-      <c r="B18" s="438" t="s">
-        <v>668</v>
-      </c>
-      <c r="C18" s="442">
+        <v>676</v>
+      </c>
+      <c r="B18" s="442" t="s">
+        <v>677</v>
+      </c>
+      <c r="C18" s="446">
         <v>15.41</v>
       </c>
       <c r="D18" s="43">
@@ -7343,23 +7380,23 @@
         <f t="shared" si="1"/>
         <v>1096.2</v>
       </c>
-      <c r="H18" s="443">
+      <c r="H18" s="447">
         <f t="shared" si="2"/>
         <v>0.464</v>
       </c>
-      <c r="I18" s="443">
+      <c r="I18" s="447">
         <f t="shared" si="3"/>
         <v>1.701</v>
       </c>
-      <c r="J18" s="443">
+      <c r="J18" s="447">
         <f t="shared" si="4"/>
         <v>9.45</v>
       </c>
-      <c r="K18" s="443">
+      <c r="K18" s="447">
         <f t="shared" si="5"/>
         <v>11.615</v>
       </c>
-      <c r="L18" s="444">
+      <c r="L18" s="448">
         <f t="shared" si="6"/>
         <v>2.165</v>
       </c>
@@ -7370,12 +7407,12 @@
     </row>
     <row r="19">
       <c r="A19" s="3" t="s">
-        <v>669</v>
-      </c>
-      <c r="B19" s="438" t="s">
-        <v>670</v>
-      </c>
-      <c r="C19" s="439">
+        <v>678</v>
+      </c>
+      <c r="B19" s="442" t="s">
+        <v>679</v>
+      </c>
+      <c r="C19" s="443">
         <v>16.16</v>
       </c>
       <c r="D19" s="43">
@@ -7391,19 +7428,19 @@
         <f t="shared" si="1"/>
         <v>1368</v>
       </c>
-      <c r="H19" s="440">
+      <c r="H19" s="444">
         <f t="shared" si="2"/>
         <v>0.384</v>
       </c>
-      <c r="I19" s="440">
+      <c r="I19" s="444">
         <f t="shared" si="3"/>
         <v>2.565</v>
       </c>
-      <c r="J19" s="440">
+      <c r="J19" s="444">
         <f t="shared" si="4"/>
         <v>9.9</v>
       </c>
-      <c r="K19" s="440">
+      <c r="K19" s="444">
         <f t="shared" si="5"/>
         <v>12.849</v>
       </c>
@@ -7418,12 +7455,12 @@
     </row>
     <row r="20">
       <c r="A20" s="3" t="s">
-        <v>671</v>
-      </c>
-      <c r="B20" s="441" t="s">
-        <v>672</v>
-      </c>
-      <c r="C20" s="439">
+        <v>680</v>
+      </c>
+      <c r="B20" s="445" t="s">
+        <v>681</v>
+      </c>
+      <c r="C20" s="443">
         <v>6.37</v>
       </c>
       <c r="D20" s="43">
@@ -7439,19 +7476,19 @@
         <f t="shared" si="1"/>
         <v>2763.6</v>
       </c>
-      <c r="H20" s="440">
+      <c r="H20" s="444">
         <f t="shared" si="2"/>
         <v>4.704</v>
       </c>
-      <c r="I20" s="440">
+      <c r="I20" s="444">
         <f t="shared" si="3"/>
         <v>0.423</v>
       </c>
-      <c r="J20" s="440">
+      <c r="J20" s="444">
         <f t="shared" si="4"/>
         <v>6.75</v>
       </c>
-      <c r="K20" s="440">
+      <c r="K20" s="444">
         <f t="shared" si="5"/>
         <v>11.877</v>
       </c>
@@ -7466,12 +7503,12 @@
     </row>
     <row r="21">
       <c r="A21" s="3" t="s">
-        <v>673</v>
-      </c>
-      <c r="B21" s="438" t="s">
-        <v>674</v>
-      </c>
-      <c r="C21" s="442">
+        <v>682</v>
+      </c>
+      <c r="B21" s="442" t="s">
+        <v>683</v>
+      </c>
+      <c r="C21" s="446">
         <v>16.17</v>
       </c>
       <c r="D21" s="43">
@@ -7487,19 +7524,19 @@
         <f t="shared" si="1"/>
         <v>4530</v>
       </c>
-      <c r="H21" s="440">
+      <c r="H21" s="444">
         <f t="shared" si="2"/>
         <v>0.48</v>
       </c>
-      <c r="I21" s="440">
+      <c r="I21" s="444">
         <f t="shared" si="3"/>
         <v>6.795</v>
       </c>
-      <c r="J21" s="440">
+      <c r="J21" s="444">
         <f t="shared" si="4"/>
         <v>12.42</v>
       </c>
-      <c r="K21" s="440">
+      <c r="K21" s="444">
         <f t="shared" si="5"/>
         <v>19.695</v>
       </c>
@@ -7514,12 +7551,12 @@
     </row>
     <row r="22">
       <c r="A22" s="3" t="s">
-        <v>675</v>
-      </c>
-      <c r="B22" s="441" t="s">
-        <v>676</v>
-      </c>
-      <c r="C22" s="439">
+        <v>684</v>
+      </c>
+      <c r="B22" s="445" t="s">
+        <v>685</v>
+      </c>
+      <c r="C22" s="443">
         <v>12.31</v>
       </c>
       <c r="D22" s="43">
@@ -7535,19 +7572,19 @@
         <f t="shared" si="1"/>
         <v>2088</v>
       </c>
-      <c r="H22" s="440">
+      <c r="H22" s="444">
         <f t="shared" si="2"/>
         <v>1.152</v>
       </c>
-      <c r="I22" s="440">
+      <c r="I22" s="444">
         <f t="shared" si="3"/>
         <v>1.305</v>
       </c>
-      <c r="J22" s="440">
+      <c r="J22" s="444">
         <f t="shared" si="4"/>
         <v>11.88</v>
       </c>
-      <c r="K22" s="440">
+      <c r="K22" s="444">
         <f t="shared" si="5"/>
         <v>14.337</v>
       </c>
@@ -7562,12 +7599,12 @@
     </row>
     <row r="23">
       <c r="A23" s="3" t="s">
-        <v>677</v>
-      </c>
-      <c r="B23" s="441" t="s">
-        <v>678</v>
-      </c>
-      <c r="C23" s="439">
+        <v>686</v>
+      </c>
+      <c r="B23" s="445" t="s">
+        <v>687</v>
+      </c>
+      <c r="C23" s="443">
         <v>5.82</v>
       </c>
       <c r="D23" s="43">
@@ -7583,19 +7620,19 @@
         <f t="shared" si="1"/>
         <v>2761.2</v>
       </c>
-      <c r="H23" s="440">
+      <c r="H23" s="444">
         <f t="shared" si="2"/>
         <v>7.488</v>
       </c>
-      <c r="I23" s="440">
+      <c r="I23" s="444">
         <f t="shared" si="3"/>
         <v>0.2655</v>
       </c>
-      <c r="J23" s="440">
+      <c r="J23" s="444">
         <f t="shared" si="4"/>
         <v>5.58</v>
       </c>
-      <c r="K23" s="440">
+      <c r="K23" s="444">
         <f t="shared" si="5"/>
         <v>13.3335</v>
       </c>
@@ -7610,12 +7647,12 @@
     </row>
     <row r="24">
       <c r="A24" s="3" t="s">
-        <v>679</v>
-      </c>
-      <c r="B24" s="438" t="s">
-        <v>680</v>
-      </c>
-      <c r="C24" s="439">
+        <v>688</v>
+      </c>
+      <c r="B24" s="442" t="s">
+        <v>689</v>
+      </c>
+      <c r="C24" s="443">
         <v>9.58</v>
       </c>
       <c r="D24" s="43">
@@ -7631,19 +7668,19 @@
         <f t="shared" si="1"/>
         <v>2875</v>
       </c>
-      <c r="H24" s="440">
+      <c r="H24" s="444">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="I24" s="440">
+      <c r="I24" s="444">
         <f t="shared" si="3"/>
         <v>1.035</v>
       </c>
-      <c r="J24" s="440">
+      <c r="J24" s="444">
         <f t="shared" si="4"/>
         <v>11.43</v>
       </c>
-      <c r="K24" s="440">
+      <c r="K24" s="444">
         <f t="shared" si="5"/>
         <v>14.465</v>
       </c>
@@ -7658,12 +7695,12 @@
     </row>
     <row r="25">
       <c r="A25" s="3" t="s">
-        <v>681</v>
-      </c>
-      <c r="B25" s="438" t="s">
-        <v>682</v>
-      </c>
-      <c r="C25" s="439">
+        <v>690</v>
+      </c>
+      <c r="B25" s="442" t="s">
+        <v>691</v>
+      </c>
+      <c r="C25" s="443">
         <v>10.78</v>
       </c>
       <c r="D25" s="43">
@@ -7679,19 +7716,19 @@
         <f t="shared" si="1"/>
         <v>2822</v>
       </c>
-      <c r="H25" s="440">
+      <c r="H25" s="444">
         <f t="shared" si="2"/>
         <v>1.328</v>
       </c>
-      <c r="I25" s="440">
+      <c r="I25" s="444">
         <f t="shared" si="3"/>
         <v>1.53</v>
       </c>
-      <c r="J25" s="440">
+      <c r="J25" s="444">
         <f t="shared" si="4"/>
         <v>14.85</v>
       </c>
-      <c r="K25" s="440">
+      <c r="K25" s="444">
         <f t="shared" si="5"/>
         <v>17.708</v>
       </c>
@@ -7706,12 +7743,12 @@
     </row>
     <row r="26">
       <c r="A26" s="3" t="s">
-        <v>683</v>
-      </c>
-      <c r="B26" s="438" t="s">
-        <v>684</v>
-      </c>
-      <c r="C26" s="442">
+        <v>692</v>
+      </c>
+      <c r="B26" s="442" t="s">
+        <v>693</v>
+      </c>
+      <c r="C26" s="446">
         <v>21.16</v>
       </c>
       <c r="D26" s="43">
@@ -7727,19 +7764,19 @@
         <f t="shared" si="1"/>
         <v>869.4</v>
       </c>
-      <c r="H26" s="440">
+      <c r="H26" s="444">
         <f t="shared" si="2"/>
         <v>0.368</v>
       </c>
-      <c r="I26" s="440">
+      <c r="I26" s="444">
         <f t="shared" si="3"/>
         <v>1.701</v>
       </c>
-      <c r="J26" s="440">
+      <c r="J26" s="444">
         <f t="shared" si="4"/>
         <v>23.76</v>
       </c>
-      <c r="K26" s="440">
+      <c r="K26" s="444">
         <f t="shared" si="5"/>
         <v>25.829</v>
       </c>
@@ -7754,12 +7791,12 @@
     </row>
     <row r="27">
       <c r="A27" s="3" t="s">
-        <v>685</v>
-      </c>
-      <c r="B27" s="438" t="s">
-        <v>686</v>
-      </c>
-      <c r="C27" s="439">
+        <v>694</v>
+      </c>
+      <c r="B27" s="442" t="s">
+        <v>695</v>
+      </c>
+      <c r="C27" s="443">
         <v>18.99</v>
       </c>
       <c r="D27" s="43">
@@ -7775,19 +7812,19 @@
         <f t="shared" si="1"/>
         <v>2583</v>
       </c>
-      <c r="H27" s="440">
+      <c r="H27" s="444">
         <f t="shared" si="2"/>
         <v>0.656</v>
       </c>
-      <c r="I27" s="440">
+      <c r="I27" s="444">
         <f t="shared" si="3"/>
         <v>2.835</v>
       </c>
-      <c r="J27" s="440">
+      <c r="J27" s="444">
         <f t="shared" si="4"/>
         <v>27</v>
       </c>
-      <c r="K27" s="440">
+      <c r="K27" s="444">
         <f t="shared" si="5"/>
         <v>30.491</v>
       </c>
@@ -7802,10 +7839,10 @@
     </row>
     <row r="28">
       <c r="A28" s="3" t="s">
-        <v>687</v>
-      </c>
-      <c r="B28" s="438" t="s">
-        <v>688</v>
+        <v>696</v>
+      </c>
+      <c r="B28" s="442" t="s">
+        <v>697</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>315</v>
@@ -7823,19 +7860,19 @@
         <f t="shared" si="1"/>
         <v>4606</v>
       </c>
-      <c r="H28" s="440">
+      <c r="H28" s="444">
         <f t="shared" si="2"/>
         <v>0.224</v>
       </c>
-      <c r="I28" s="440">
+      <c r="I28" s="444">
         <f t="shared" si="3"/>
         <v>14.805</v>
       </c>
-      <c r="J28" s="440">
+      <c r="J28" s="444">
         <f t="shared" si="4"/>
         <v>29.88</v>
       </c>
-      <c r="K28" s="440">
+      <c r="K28" s="444">
         <f t="shared" si="5"/>
         <v>44.909</v>
       </c>
@@ -7850,12 +7887,12 @@
     </row>
     <row r="29">
       <c r="A29" s="3" t="s">
-        <v>689</v>
-      </c>
-      <c r="B29" s="441" t="s">
-        <v>690</v>
-      </c>
-      <c r="C29" s="439">
+        <v>698</v>
+      </c>
+      <c r="B29" s="445" t="s">
+        <v>699</v>
+      </c>
+      <c r="C29" s="443">
         <v>35.41</v>
       </c>
       <c r="D29" s="43">
@@ -7871,19 +7908,19 @@
         <f t="shared" si="1"/>
         <v>1521.5</v>
       </c>
-      <c r="H29" s="440">
+      <c r="H29" s="444">
         <f t="shared" si="2"/>
         <v>0.136</v>
       </c>
-      <c r="I29" s="440">
+      <c r="I29" s="444">
         <f t="shared" si="3"/>
         <v>8.055</v>
       </c>
-      <c r="J29" s="440">
+      <c r="J29" s="444">
         <f t="shared" si="4"/>
         <v>32.58</v>
       </c>
-      <c r="K29" s="440">
+      <c r="K29" s="444">
         <f t="shared" si="5"/>
         <v>40.771</v>
       </c>
@@ -7898,12 +7935,12 @@
     </row>
     <row r="30">
       <c r="A30" s="3" t="s">
-        <v>691</v>
-      </c>
-      <c r="B30" s="441" t="s">
-        <v>692</v>
-      </c>
-      <c r="C30" s="439">
+        <v>700</v>
+      </c>
+      <c r="B30" s="445" t="s">
+        <v>701</v>
+      </c>
+      <c r="C30" s="443">
         <v>5.69</v>
       </c>
       <c r="D30" s="43">
@@ -7919,19 +7956,19 @@
         <f t="shared" si="1"/>
         <v>6270</v>
       </c>
-      <c r="H30" s="440">
+      <c r="H30" s="444">
         <f t="shared" si="2"/>
         <v>1.52</v>
       </c>
-      <c r="I30" s="440">
+      <c r="I30" s="444">
         <f t="shared" si="3"/>
         <v>2.97</v>
       </c>
-      <c r="J30" s="440">
+      <c r="J30" s="444">
         <f t="shared" si="4"/>
         <v>33.48</v>
       </c>
-      <c r="K30" s="440">
+      <c r="K30" s="444">
         <f t="shared" si="5"/>
         <v>37.97</v>
       </c>
@@ -7946,12 +7983,12 @@
     </row>
     <row r="31">
       <c r="A31" s="3" t="s">
-        <v>693</v>
-      </c>
-      <c r="B31" s="441" t="s">
-        <v>694</v>
-      </c>
-      <c r="C31" s="442">
+        <v>702</v>
+      </c>
+      <c r="B31" s="445" t="s">
+        <v>703</v>
+      </c>
+      <c r="C31" s="446">
         <v>34.44</v>
       </c>
       <c r="D31" s="43">
@@ -7967,19 +8004,19 @@
         <f t="shared" si="1"/>
         <v>1501.5</v>
       </c>
-      <c r="H31" s="440">
+      <c r="H31" s="444">
         <f t="shared" si="2"/>
         <v>0.1232</v>
       </c>
-      <c r="I31" s="440">
+      <c r="I31" s="444">
         <f t="shared" si="3"/>
         <v>8.775</v>
       </c>
-      <c r="J31" s="440">
+      <c r="J31" s="444">
         <f t="shared" si="4"/>
         <v>76.5</v>
       </c>
-      <c r="K31" s="440">
+      <c r="K31" s="444">
         <f t="shared" si="5"/>
         <v>85.3982</v>
       </c>
@@ -7994,12 +8031,12 @@
     </row>
     <row r="32">
       <c r="A32" s="3" t="s">
-        <v>695</v>
-      </c>
-      <c r="B32" s="438" t="s">
-        <v>696</v>
-      </c>
-      <c r="C32" s="439">
+        <v>704</v>
+      </c>
+      <c r="B32" s="442" t="s">
+        <v>705</v>
+      </c>
+      <c r="C32" s="443">
         <v>0.846</v>
       </c>
       <c r="D32" s="43">
@@ -8015,19 +8052,19 @@
         <f t="shared" si="1"/>
         <v>4920</v>
       </c>
-      <c r="H32" s="440">
+      <c r="H32" s="444">
         <f t="shared" si="2"/>
         <v>4.8</v>
       </c>
-      <c r="I32" s="440">
+      <c r="I32" s="444">
         <f t="shared" si="3"/>
         <v>0.738</v>
       </c>
-      <c r="J32" s="440">
+      <c r="J32" s="444">
         <f t="shared" si="4"/>
         <v>90</v>
       </c>
-      <c r="K32" s="440">
+      <c r="K32" s="444">
         <f t="shared" si="5"/>
         <v>95.538</v>
       </c>
@@ -8042,12 +8079,12 @@
     </row>
     <row r="33">
       <c r="A33" s="3" t="s">
-        <v>697</v>
-      </c>
-      <c r="B33" s="438" t="s">
-        <v>698</v>
-      </c>
-      <c r="C33" s="439">
+        <v>706</v>
+      </c>
+      <c r="B33" s="442" t="s">
+        <v>707</v>
+      </c>
+      <c r="C33" s="443">
         <v>5.86</v>
       </c>
       <c r="D33" s="43">
@@ -8057,25 +8094,25 @@
         <v>11.0</v>
       </c>
       <c r="F33" s="43" t="s">
-        <v>699</v>
+        <v>708</v>
       </c>
       <c r="G33" s="25">
         <f t="shared" si="1"/>
         <v>4950</v>
       </c>
-      <c r="H33" s="440">
+      <c r="H33" s="444">
         <f t="shared" si="2"/>
         <v>7.2</v>
       </c>
-      <c r="I33" s="440">
+      <c r="I33" s="444">
         <f t="shared" si="3"/>
         <v>0.495</v>
       </c>
-      <c r="J33" s="440" t="str">
+      <c r="J33" s="444" t="str">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K33" s="440" t="str">
+      <c r="K33" s="444" t="str">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
@@ -8090,12 +8127,12 @@
     </row>
     <row r="34">
       <c r="A34" s="3" t="s">
-        <v>700</v>
-      </c>
-      <c r="B34" s="438" t="s">
-        <v>701</v>
-      </c>
-      <c r="C34" s="439">
+        <v>709</v>
+      </c>
+      <c r="B34" s="442" t="s">
+        <v>710</v>
+      </c>
+      <c r="C34" s="443">
         <v>6.45</v>
       </c>
       <c r="D34" s="43">
@@ -8105,25 +8142,25 @@
         <v>11.0</v>
       </c>
       <c r="F34" s="43" t="s">
-        <v>699</v>
+        <v>708</v>
       </c>
       <c r="G34" s="25">
         <f t="shared" si="1"/>
         <v>8250</v>
       </c>
-      <c r="H34" s="440">
+      <c r="H34" s="444">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="I34" s="440">
+      <c r="I34" s="444">
         <f t="shared" si="3"/>
         <v>0.495</v>
       </c>
-      <c r="J34" s="440" t="str">
+      <c r="J34" s="444" t="str">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K34" s="440" t="str">
+      <c r="K34" s="444" t="str">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
@@ -8138,12 +8175,12 @@
     </row>
     <row r="35">
       <c r="A35" s="3" t="s">
-        <v>702</v>
-      </c>
-      <c r="B35" s="441" t="s">
-        <v>703</v>
-      </c>
-      <c r="C35" s="439">
+        <v>711</v>
+      </c>
+      <c r="B35" s="445" t="s">
+        <v>712</v>
+      </c>
+      <c r="C35" s="443">
         <v>4.58</v>
       </c>
       <c r="D35" s="43">
@@ -8153,25 +8190,25 @@
         <v>5.0</v>
       </c>
       <c r="F35" s="43" t="s">
-        <v>699</v>
+        <v>708</v>
       </c>
       <c r="G35" s="25">
         <f t="shared" si="1"/>
         <v>5000</v>
       </c>
-      <c r="H35" s="440">
+      <c r="H35" s="444">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="I35" s="440">
+      <c r="I35" s="444">
         <f t="shared" si="3"/>
         <v>0.225</v>
       </c>
-      <c r="J35" s="440" t="str">
+      <c r="J35" s="444" t="str">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K35" s="440" t="str">
+      <c r="K35" s="444" t="str">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
@@ -8185,72 +8222,72 @@
       </c>
     </row>
     <row r="36">
-      <c r="B36" s="445"/>
+      <c r="B36" s="449"/>
     </row>
     <row r="37">
-      <c r="B37" s="445"/>
+      <c r="B37" s="449"/>
     </row>
     <row r="38">
       <c r="A38" s="7" t="s">
-        <v>704</v>
+        <v>713</v>
       </c>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="7"/>
     </row>
     <row r="39">
-      <c r="A39" s="429" t="s">
-        <v>627</v>
-      </c>
-      <c r="B39" s="430">
+      <c r="A39" s="433" t="s">
+        <v>636</v>
+      </c>
+      <c r="B39" s="434">
         <v>1.0</v>
       </c>
-      <c r="C39" s="431" t="s">
+      <c r="C39" s="435" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="432" t="s">
-        <v>628</v>
+      <c r="A40" s="436" t="s">
+        <v>637</v>
       </c>
       <c r="B40" s="3">
         <v>30.0</v>
       </c>
-      <c r="C40" s="433" t="s">
-        <v>629</v>
+      <c r="C40" s="437" t="s">
+        <v>638</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="432" t="s">
-        <v>630</v>
+      <c r="A41" s="436" t="s">
+        <v>639</v>
       </c>
       <c r="B41" s="3">
         <v>190.0</v>
       </c>
-      <c r="C41" s="433" t="s">
+      <c r="C41" s="437" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="432" t="s">
-        <v>631</v>
+      <c r="A42" s="436" t="s">
+        <v>640</v>
       </c>
       <c r="B42" s="18">
         <v>4.0</v>
       </c>
-      <c r="C42" s="433" t="s">
+      <c r="C42" s="437" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="434" t="s">
-        <v>632</v>
-      </c>
-      <c r="B43" s="435">
+      <c r="A43" s="438" t="s">
+        <v>641</v>
+      </c>
+      <c r="B43" s="439">
         <v>0.5</v>
       </c>
-      <c r="C43" s="436" t="s">
-        <v>633</v>
+      <c r="C43" s="440" t="s">
+        <v>642</v>
       </c>
     </row>
     <row r="44">
@@ -8260,79 +8297,79 @@
     </row>
     <row r="45">
       <c r="A45" s="40" t="s">
-        <v>634</v>
+        <v>643</v>
       </c>
       <c r="B45" s="40" t="s">
-        <v>635</v>
+        <v>644</v>
       </c>
       <c r="C45" s="40" t="s">
-        <v>636</v>
+        <v>645</v>
       </c>
       <c r="D45" s="40" t="s">
-        <v>705</v>
+        <v>714</v>
       </c>
       <c r="E45" s="40" t="s">
-        <v>706</v>
+        <v>715</v>
       </c>
       <c r="F45" s="40" t="s">
-        <v>707</v>
+        <v>716</v>
       </c>
       <c r="G45" s="40" t="s">
-        <v>708</v>
+        <v>717</v>
       </c>
       <c r="H45" s="40" t="s">
-        <v>709</v>
+        <v>718</v>
       </c>
       <c r="I45" s="40" t="s">
-        <v>637</v>
+        <v>646</v>
       </c>
       <c r="J45" s="40" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="K45" s="40" t="s">
-        <v>639</v>
+        <v>648</v>
       </c>
       <c r="L45" s="40" t="s">
-        <v>640</v>
-      </c>
-      <c r="M45" s="446" t="s">
-        <v>641</v>
-      </c>
-      <c r="N45" s="446" t="s">
-        <v>642</v>
-      </c>
-      <c r="O45" s="446" t="s">
-        <v>643</v>
-      </c>
-      <c r="P45" s="446" t="s">
-        <v>644</v>
-      </c>
-      <c r="Q45" s="437"/>
-      <c r="R45" s="437"/>
-      <c r="S45" s="437"/>
-      <c r="T45" s="437"/>
-      <c r="U45" s="437"/>
-      <c r="V45" s="437"/>
-      <c r="W45" s="437"/>
-      <c r="X45" s="437"/>
-      <c r="Y45" s="437"/>
-      <c r="Z45" s="437"/>
+        <v>649</v>
+      </c>
+      <c r="M45" s="450" t="s">
+        <v>650</v>
+      </c>
+      <c r="N45" s="450" t="s">
+        <v>651</v>
+      </c>
+      <c r="O45" s="450" t="s">
+        <v>652</v>
+      </c>
+      <c r="P45" s="450" t="s">
+        <v>653</v>
+      </c>
+      <c r="Q45" s="441"/>
+      <c r="R45" s="441"/>
+      <c r="S45" s="441"/>
+      <c r="T45" s="441"/>
+      <c r="U45" s="441"/>
+      <c r="V45" s="441"/>
+      <c r="W45" s="441"/>
+      <c r="X45" s="441"/>
+      <c r="Y45" s="441"/>
+      <c r="Z45" s="441"/>
     </row>
     <row r="46">
       <c r="A46" s="3" t="s">
-        <v>710</v>
-      </c>
-      <c r="B46" s="447" t="s">
-        <v>711</v>
-      </c>
-      <c r="C46" s="442">
+        <v>719</v>
+      </c>
+      <c r="B46" s="451" t="s">
+        <v>720</v>
+      </c>
+      <c r="C46" s="446">
         <v>2.96</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>712</v>
+        <v>721</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>713</v>
+        <v>722</v>
       </c>
       <c r="F46" s="43">
         <v>80.0</v>
@@ -8356,38 +8393,38 @@
         <f t="shared" ref="L46:L78" si="8">I46*J46</f>
         <v>72.93</v>
       </c>
-      <c r="M46" s="440">
+      <c r="M46" s="444">
         <f t="shared" ref="M46:M78" si="9">I46/1000*$B$40^2</f>
         <v>1.287</v>
       </c>
-      <c r="N46" s="440">
+      <c r="N46" s="444">
         <f t="shared" ref="N46:N78" si="10">($B$39*$B$40*$B$41*1000*(J46*10^-9)/$B$42)*$B$43</f>
         <v>0.0363375</v>
       </c>
-      <c r="O46" s="440">
+      <c r="O46" s="444">
         <f t="shared" ref="O46:O78" si="11">K46*10^-9*$B$39*$B$41*1000</f>
         <v>0.0551</v>
       </c>
-      <c r="P46" s="440">
+      <c r="P46" s="444">
         <f t="shared" ref="P46:P78" si="12">M46+N46+O46</f>
         <v>1.3784375</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="3" t="s">
-        <v>714</v>
-      </c>
-      <c r="B47" s="447" t="s">
-        <v>715</v>
-      </c>
-      <c r="C47" s="442">
+        <v>723</v>
+      </c>
+      <c r="B47" s="451" t="s">
+        <v>724</v>
+      </c>
+      <c r="C47" s="446">
         <v>3.26</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>716</v>
+        <v>725</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>713</v>
+        <v>722</v>
       </c>
       <c r="F47" s="43">
         <v>60.0</v>
@@ -8411,19 +8448,19 @@
         <f t="shared" si="8"/>
         <v>139.5</v>
       </c>
-      <c r="M47" s="440">
+      <c r="M47" s="444">
         <f t="shared" si="9"/>
         <v>1.395</v>
       </c>
-      <c r="N47" s="440">
+      <c r="N47" s="444">
         <f t="shared" si="10"/>
         <v>0.064125</v>
       </c>
-      <c r="O47" s="440">
+      <c r="O47" s="444">
         <f t="shared" si="11"/>
         <v>0.00798</v>
       </c>
-      <c r="P47" s="440">
+      <c r="P47" s="444">
         <f t="shared" si="12"/>
         <v>1.467105</v>
       </c>
@@ -8432,17 +8469,17 @@
       <c r="A48" s="7" t="s">
         <v>439</v>
       </c>
-      <c r="B48" s="447" t="s">
-        <v>717</v>
-      </c>
-      <c r="C48" s="442">
+      <c r="B48" s="451" t="s">
+        <v>726</v>
+      </c>
+      <c r="C48" s="446">
         <v>2.63</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>716</v>
+        <v>725</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>713</v>
+        <v>722</v>
       </c>
       <c r="F48" s="43">
         <v>60.0</v>
@@ -8466,38 +8503,38 @@
         <f t="shared" si="8"/>
         <v>69</v>
       </c>
-      <c r="M48" s="440">
+      <c r="M48" s="444">
         <f t="shared" si="9"/>
         <v>2.07</v>
       </c>
-      <c r="N48" s="440">
+      <c r="N48" s="444">
         <f t="shared" si="10"/>
         <v>0.021375</v>
       </c>
-      <c r="O48" s="440">
+      <c r="O48" s="444">
         <f t="shared" si="11"/>
         <v>0.00684</v>
       </c>
-      <c r="P48" s="440">
+      <c r="P48" s="444">
         <f t="shared" si="12"/>
         <v>2.098215</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="7" t="s">
-        <v>718</v>
-      </c>
-      <c r="B49" s="447" t="s">
-        <v>719</v>
-      </c>
-      <c r="C49" s="442">
+        <v>727</v>
+      </c>
+      <c r="B49" s="451" t="s">
+        <v>728</v>
+      </c>
+      <c r="C49" s="446">
         <v>3.42</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>720</v>
+        <v>729</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>721</v>
+        <v>730</v>
       </c>
       <c r="F49" s="43">
         <v>100.0</v>
@@ -8521,38 +8558,38 @@
         <f t="shared" si="8"/>
         <v>22.08</v>
       </c>
-      <c r="M49" s="440">
+      <c r="M49" s="444">
         <f t="shared" si="9"/>
         <v>2.16</v>
       </c>
-      <c r="N49" s="440">
+      <c r="N49" s="444">
         <f t="shared" si="10"/>
         <v>0.006555</v>
       </c>
-      <c r="O49" s="440">
+      <c r="O49" s="444">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="P49" s="440">
+      <c r="P49" s="444">
         <f t="shared" si="12"/>
         <v>2.166555</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="3" t="s">
+        <v>731</v>
+      </c>
+      <c r="B50" s="451" t="s">
+        <v>732</v>
+      </c>
+      <c r="C50" s="446">
+        <v>1.46</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>733</v>
+      </c>
+      <c r="E50" s="3" t="s">
         <v>722</v>
-      </c>
-      <c r="B50" s="447" t="s">
-        <v>723</v>
-      </c>
-      <c r="C50" s="442">
-        <v>1.46</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>724</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>713</v>
       </c>
       <c r="F50" s="43">
         <v>60.0</v>
@@ -8576,38 +8613,38 @@
         <f t="shared" si="8"/>
         <v>124.8</v>
       </c>
-      <c r="M50" s="440">
+      <c r="M50" s="444">
         <f t="shared" si="9"/>
         <v>2.16</v>
       </c>
-      <c r="N50" s="440">
+      <c r="N50" s="444">
         <f t="shared" si="10"/>
         <v>0.03705</v>
       </c>
-      <c r="O50" s="440">
+      <c r="O50" s="444">
         <f t="shared" si="11"/>
         <v>0.0114</v>
       </c>
-      <c r="P50" s="440">
+      <c r="P50" s="444">
         <f t="shared" si="12"/>
         <v>2.20845</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="3" t="s">
-        <v>725</v>
-      </c>
-      <c r="B51" s="447" t="s">
-        <v>726</v>
-      </c>
-      <c r="C51" s="442">
+        <v>734</v>
+      </c>
+      <c r="B51" s="451" t="s">
+        <v>735</v>
+      </c>
+      <c r="C51" s="446">
         <v>2.32</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>727</v>
+        <v>736</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>713</v>
+        <v>722</v>
       </c>
       <c r="F51" s="43">
         <v>60.0</v>
@@ -8631,38 +8668,38 @@
         <f t="shared" si="8"/>
         <v>100</v>
       </c>
-      <c r="M51" s="440">
+      <c r="M51" s="444">
         <f t="shared" si="9"/>
         <v>2.25</v>
       </c>
-      <c r="N51" s="440">
+      <c r="N51" s="444">
         <f t="shared" si="10"/>
         <v>0.0285</v>
       </c>
-      <c r="O51" s="440">
+      <c r="O51" s="444">
         <f t="shared" si="11"/>
         <v>0.007258</v>
       </c>
-      <c r="P51" s="440">
+      <c r="P51" s="444">
         <f t="shared" si="12"/>
         <v>2.285758</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="3" t="s">
-        <v>728</v>
-      </c>
-      <c r="B52" s="438" t="s">
-        <v>729</v>
-      </c>
-      <c r="C52" s="442">
+        <v>737</v>
+      </c>
+      <c r="B52" s="442" t="s">
+        <v>738</v>
+      </c>
+      <c r="C52" s="446">
         <v>1.3</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>730</v>
+        <v>739</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>713</v>
+        <v>722</v>
       </c>
       <c r="F52" s="43">
         <v>60.0</v>
@@ -8686,38 +8723,38 @@
         <f t="shared" si="8"/>
         <v>177.5</v>
       </c>
-      <c r="M52" s="440">
+      <c r="M52" s="444">
         <f t="shared" si="9"/>
         <v>2.25</v>
       </c>
-      <c r="N52" s="440">
+      <c r="N52" s="444">
         <f t="shared" si="10"/>
         <v>0.0505875</v>
       </c>
-      <c r="O52" s="440">
+      <c r="O52" s="444">
         <f t="shared" si="11"/>
         <v>0.00969</v>
       </c>
-      <c r="P52" s="440">
+      <c r="P52" s="444">
         <f t="shared" si="12"/>
         <v>2.3102775</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="3" t="s">
-        <v>731</v>
-      </c>
-      <c r="B53" s="447" t="s">
-        <v>732</v>
-      </c>
-      <c r="C53" s="442">
+        <v>740</v>
+      </c>
+      <c r="B53" s="451" t="s">
+        <v>741</v>
+      </c>
+      <c r="C53" s="446">
         <v>3.93</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>716</v>
+        <v>725</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>713</v>
+        <v>722</v>
       </c>
       <c r="F53" s="43">
         <v>80.0</v>
@@ -8741,38 +8778,38 @@
         <f t="shared" si="8"/>
         <v>86.7</v>
       </c>
-      <c r="M53" s="440">
+      <c r="M53" s="444">
         <f t="shared" si="9"/>
         <v>2.295</v>
       </c>
-      <c r="N53" s="440">
+      <c r="N53" s="444">
         <f t="shared" si="10"/>
         <v>0.024225</v>
       </c>
-      <c r="O53" s="440">
+      <c r="O53" s="444">
         <f t="shared" si="11"/>
         <v>0.01083</v>
       </c>
-      <c r="P53" s="440">
+      <c r="P53" s="444">
         <f t="shared" si="12"/>
         <v>2.330055</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="3" t="s">
-        <v>733</v>
-      </c>
-      <c r="B54" s="448" t="s">
-        <v>734</v>
-      </c>
-      <c r="C54" s="442">
+        <v>742</v>
+      </c>
+      <c r="B54" s="452" t="s">
+        <v>743</v>
+      </c>
+      <c r="C54" s="446">
         <v>1.62</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>735</v>
+        <v>744</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>713</v>
+        <v>722</v>
       </c>
       <c r="F54" s="43">
         <v>80.0</v>
@@ -8796,38 +8833,38 @@
         <f t="shared" si="8"/>
         <v>72.8</v>
       </c>
-      <c r="M54" s="440">
+      <c r="M54" s="444">
         <f t="shared" si="9"/>
         <v>2.34</v>
       </c>
-      <c r="N54" s="440">
+      <c r="N54" s="444">
         <f t="shared" si="10"/>
         <v>0.01995</v>
       </c>
-      <c r="O54" s="440">
+      <c r="O54" s="444">
         <f t="shared" si="11"/>
         <v>0.03097</v>
       </c>
-      <c r="P54" s="440">
+      <c r="P54" s="444">
         <f t="shared" si="12"/>
         <v>2.39092</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="3" t="s">
-        <v>736</v>
-      </c>
-      <c r="B55" s="447" t="s">
-        <v>737</v>
-      </c>
-      <c r="C55" s="442">
+        <v>745</v>
+      </c>
+      <c r="B55" s="451" t="s">
+        <v>746</v>
+      </c>
+      <c r="C55" s="446">
         <v>1.62</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>716</v>
+        <v>725</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>713</v>
+        <v>722</v>
       </c>
       <c r="F55" s="43">
         <v>60.0</v>
@@ -8851,38 +8888,38 @@
         <f t="shared" si="8"/>
         <v>81</v>
       </c>
-      <c r="M55" s="440">
+      <c r="M55" s="444">
         <f t="shared" si="9"/>
         <v>2.43</v>
       </c>
-      <c r="N55" s="440">
+      <c r="N55" s="444">
         <f t="shared" si="10"/>
         <v>0.021375</v>
       </c>
-      <c r="O55" s="440">
+      <c r="O55" s="444">
         <f t="shared" si="11"/>
         <v>0.00684</v>
       </c>
-      <c r="P55" s="440">
+      <c r="P55" s="444">
         <f t="shared" si="12"/>
         <v>2.458215</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="3" t="s">
-        <v>738</v>
-      </c>
-      <c r="B56" s="448" t="s">
-        <v>739</v>
-      </c>
-      <c r="C56" s="442">
+        <v>747</v>
+      </c>
+      <c r="B56" s="452" t="s">
+        <v>748</v>
+      </c>
+      <c r="C56" s="446">
         <v>1.5</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>740</v>
+        <v>749</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>713</v>
+        <v>722</v>
       </c>
       <c r="F56" s="43">
         <v>60.0</v>
@@ -8906,38 +8943,38 @@
         <f t="shared" si="8"/>
         <v>58.8</v>
       </c>
-      <c r="M56" s="440">
+      <c r="M56" s="444">
         <f t="shared" si="9"/>
         <v>2.52</v>
       </c>
-      <c r="N56" s="440">
+      <c r="N56" s="444">
         <f t="shared" si="10"/>
         <v>0.0149625</v>
       </c>
-      <c r="O56" s="440">
+      <c r="O56" s="444">
         <f t="shared" si="11"/>
         <v>0.00931</v>
       </c>
-      <c r="P56" s="440">
+      <c r="P56" s="444">
         <f t="shared" si="12"/>
         <v>2.5442725</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="3" t="s">
-        <v>741</v>
-      </c>
-      <c r="B57" s="447" t="s">
-        <v>742</v>
-      </c>
-      <c r="C57" s="442">
+        <v>750</v>
+      </c>
+      <c r="B57" s="451" t="s">
+        <v>751</v>
+      </c>
+      <c r="C57" s="446">
         <v>2.26</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>716</v>
+        <v>725</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>713</v>
+        <v>722</v>
       </c>
       <c r="F57" s="43">
         <v>60.0</v>
@@ -8961,38 +8998,38 @@
         <f t="shared" si="8"/>
         <v>103.6</v>
       </c>
-      <c r="M57" s="440">
+      <c r="M57" s="444">
         <f t="shared" si="9"/>
         <v>2.52</v>
       </c>
-      <c r="N57" s="440">
+      <c r="N57" s="444">
         <f t="shared" si="10"/>
         <v>0.0263625</v>
       </c>
-      <c r="O57" s="440">
+      <c r="O57" s="444">
         <f t="shared" si="11"/>
         <v>0.00551</v>
       </c>
-      <c r="P57" s="440">
+      <c r="P57" s="444">
         <f t="shared" si="12"/>
         <v>2.5518725</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="3" t="s">
-        <v>743</v>
-      </c>
-      <c r="B58" s="438" t="s">
-        <v>744</v>
-      </c>
-      <c r="C58" s="442">
+        <v>752</v>
+      </c>
+      <c r="B58" s="442" t="s">
+        <v>753</v>
+      </c>
+      <c r="C58" s="446">
         <v>1.41</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>745</v>
+        <v>754</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>713</v>
+        <v>722</v>
       </c>
       <c r="F58" s="43">
         <v>60.0</v>
@@ -9016,38 +9053,38 @@
         <f t="shared" si="8"/>
         <v>168</v>
       </c>
-      <c r="M58" s="440">
+      <c r="M58" s="444">
         <f t="shared" si="9"/>
         <v>2.7</v>
       </c>
-      <c r="N58" s="440">
+      <c r="N58" s="444">
         <f t="shared" si="10"/>
         <v>0.0399</v>
       </c>
-      <c r="O58" s="440">
+      <c r="O58" s="444">
         <f t="shared" si="11"/>
         <v>0.01216</v>
       </c>
-      <c r="P58" s="440">
+      <c r="P58" s="444">
         <f t="shared" si="12"/>
         <v>2.75206</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="3" t="s">
-        <v>746</v>
-      </c>
-      <c r="B59" s="447" t="s">
-        <v>747</v>
-      </c>
-      <c r="C59" s="442">
+        <v>755</v>
+      </c>
+      <c r="B59" s="451" t="s">
+        <v>756</v>
+      </c>
+      <c r="C59" s="446">
         <v>1.93</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>748</v>
+        <v>757</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>713</v>
+        <v>722</v>
       </c>
       <c r="F59" s="43">
         <v>80.0</v>
@@ -9071,38 +9108,38 @@
         <f t="shared" si="8"/>
         <v>114</v>
       </c>
-      <c r="M59" s="440">
+      <c r="M59" s="444">
         <f t="shared" si="9"/>
         <v>2.7</v>
       </c>
-      <c r="N59" s="440">
+      <c r="N59" s="444">
         <f t="shared" si="10"/>
         <v>0.027075</v>
       </c>
-      <c r="O59" s="440">
+      <c r="O59" s="444">
         <f t="shared" si="11"/>
         <v>0.0285</v>
       </c>
-      <c r="P59" s="440">
+      <c r="P59" s="444">
         <f t="shared" si="12"/>
         <v>2.755575</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="3" t="s">
-        <v>749</v>
-      </c>
-      <c r="B60" s="447" t="s">
-        <v>750</v>
-      </c>
-      <c r="C60" s="442">
+        <v>758</v>
+      </c>
+      <c r="B60" s="451" t="s">
+        <v>759</v>
+      </c>
+      <c r="C60" s="446">
         <v>1.16</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>751</v>
+        <v>760</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>713</v>
+        <v>722</v>
       </c>
       <c r="F60" s="43">
         <v>80.0</v>
@@ -9126,38 +9163,38 @@
         <f t="shared" si="8"/>
         <v>55.8</v>
       </c>
-      <c r="M60" s="440">
+      <c r="M60" s="444">
         <f t="shared" si="9"/>
         <v>2.79</v>
       </c>
-      <c r="N60" s="440">
+      <c r="N60" s="444">
         <f t="shared" si="10"/>
         <v>0.012825</v>
       </c>
-      <c r="O60" s="440">
+      <c r="O60" s="444">
         <f t="shared" si="11"/>
         <v>0.01064</v>
       </c>
-      <c r="P60" s="440">
+      <c r="P60" s="444">
         <f t="shared" si="12"/>
         <v>2.813465</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="3" t="s">
-        <v>752</v>
-      </c>
-      <c r="B61" s="447" t="s">
-        <v>753</v>
-      </c>
-      <c r="C61" s="442">
+        <v>761</v>
+      </c>
+      <c r="B61" s="451" t="s">
+        <v>762</v>
+      </c>
+      <c r="C61" s="446">
         <v>7.15</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>754</v>
+        <v>763</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>721</v>
+        <v>730</v>
       </c>
       <c r="F61" s="43">
         <v>150.0</v>
@@ -9181,38 +9218,38 @@
         <f t="shared" si="8"/>
         <v>64</v>
       </c>
-      <c r="M61" s="440">
+      <c r="M61" s="444">
         <f t="shared" si="9"/>
         <v>2.88</v>
       </c>
-      <c r="N61" s="440">
+      <c r="N61" s="444">
         <f t="shared" si="10"/>
         <v>0.01425</v>
       </c>
-      <c r="O61" s="440">
+      <c r="O61" s="444">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="P61" s="440">
+      <c r="P61" s="444">
         <f t="shared" si="12"/>
         <v>2.89425</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="3" t="s">
-        <v>755</v>
-      </c>
-      <c r="B62" s="447" t="s">
-        <v>756</v>
-      </c>
-      <c r="C62" s="442">
+        <v>764</v>
+      </c>
+      <c r="B62" s="451" t="s">
+        <v>765</v>
+      </c>
+      <c r="C62" s="446">
         <v>1.64</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>757</v>
+        <v>766</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>713</v>
+        <v>722</v>
       </c>
       <c r="F62" s="43">
         <v>60.0</v>
@@ -9236,38 +9273,38 @@
         <f t="shared" si="8"/>
         <v>126.72</v>
       </c>
-      <c r="M62" s="440">
+      <c r="M62" s="444">
         <f t="shared" si="9"/>
         <v>2.88</v>
       </c>
-      <c r="N62" s="440">
+      <c r="N62" s="444">
         <f t="shared" si="10"/>
         <v>0.028215</v>
       </c>
-      <c r="O62" s="440">
+      <c r="O62" s="444">
         <f t="shared" si="11"/>
         <v>0.00722</v>
       </c>
-      <c r="P62" s="440">
+      <c r="P62" s="444">
         <f t="shared" si="12"/>
         <v>2.915435</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="3" t="s">
-        <v>758</v>
-      </c>
-      <c r="B63" s="438" t="s">
-        <v>759</v>
-      </c>
-      <c r="C63" s="442">
+        <v>767</v>
+      </c>
+      <c r="B63" s="442" t="s">
+        <v>768</v>
+      </c>
+      <c r="C63" s="446">
         <v>1.09</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>724</v>
+        <v>733</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>713</v>
+        <v>722</v>
       </c>
       <c r="F63" s="43">
         <v>60.0</v>
@@ -9291,38 +9328,38 @@
         <f t="shared" si="8"/>
         <v>112.2</v>
       </c>
-      <c r="M63" s="440">
+      <c r="M63" s="444">
         <f t="shared" si="9"/>
         <v>2.97</v>
       </c>
-      <c r="N63" s="440">
+      <c r="N63" s="444">
         <f t="shared" si="10"/>
         <v>0.024225</v>
       </c>
-      <c r="O63" s="440">
+      <c r="O63" s="444">
         <f t="shared" si="11"/>
         <v>0.00608</v>
       </c>
-      <c r="P63" s="440">
+      <c r="P63" s="444">
         <f t="shared" si="12"/>
         <v>3.000305</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="3" t="s">
-        <v>760</v>
-      </c>
-      <c r="B64" s="447" t="s">
-        <v>761</v>
-      </c>
-      <c r="C64" s="442">
+        <v>769</v>
+      </c>
+      <c r="B64" s="451" t="s">
+        <v>770</v>
+      </c>
+      <c r="C64" s="446">
         <v>1.2</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>716</v>
+        <v>725</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>713</v>
+        <v>722</v>
       </c>
       <c r="F64" s="43">
         <v>60.0</v>
@@ -9346,38 +9383,38 @@
         <f t="shared" si="8"/>
         <v>112.2</v>
       </c>
-      <c r="M64" s="440">
+      <c r="M64" s="444">
         <f t="shared" si="9"/>
         <v>3.06</v>
       </c>
-      <c r="N64" s="440">
+      <c r="N64" s="444">
         <f t="shared" si="10"/>
         <v>0.0235125</v>
       </c>
-      <c r="O64" s="440">
+      <c r="O64" s="444">
         <f t="shared" si="11"/>
         <v>0.01235</v>
       </c>
-      <c r="P64" s="440">
+      <c r="P64" s="444">
         <f t="shared" si="12"/>
         <v>3.0958625</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="3" t="s">
-        <v>762</v>
-      </c>
-      <c r="B65" s="447" t="s">
-        <v>763</v>
-      </c>
-      <c r="C65" s="442">
+        <v>771</v>
+      </c>
+      <c r="B65" s="451" t="s">
+        <v>772</v>
+      </c>
+      <c r="C65" s="446">
         <v>2.59</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>716</v>
+        <v>725</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>713</v>
+        <v>722</v>
       </c>
       <c r="F65" s="43">
         <v>100.0</v>
@@ -9401,38 +9438,38 @@
         <f t="shared" si="8"/>
         <v>156.4</v>
       </c>
-      <c r="M65" s="440">
+      <c r="M65" s="444">
         <f t="shared" si="9"/>
         <v>3.06</v>
       </c>
-      <c r="N65" s="440">
+      <c r="N65" s="444">
         <f t="shared" si="10"/>
         <v>0.032775</v>
       </c>
-      <c r="O65" s="440">
+      <c r="O65" s="444">
         <f t="shared" si="11"/>
         <v>0.00798</v>
       </c>
-      <c r="P65" s="440">
+      <c r="P65" s="444">
         <f t="shared" si="12"/>
         <v>3.100755</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="7" t="s">
-        <v>764</v>
-      </c>
-      <c r="B66" s="448" t="s">
-        <v>765</v>
-      </c>
-      <c r="C66" s="442">
+        <v>773</v>
+      </c>
+      <c r="B66" s="452" t="s">
+        <v>774</v>
+      </c>
+      <c r="C66" s="446">
         <v>3.94</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>766</v>
+        <v>775</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>713</v>
+        <v>722</v>
       </c>
       <c r="F66" s="43">
         <v>100.0</v>
@@ -9456,38 +9493,38 @@
         <f t="shared" si="8"/>
         <v>255</v>
       </c>
-      <c r="M66" s="440">
+      <c r="M66" s="444">
         <f t="shared" si="9"/>
         <v>3.06</v>
       </c>
-      <c r="N66" s="440">
+      <c r="N66" s="444">
         <f t="shared" si="10"/>
         <v>0.0534375</v>
       </c>
-      <c r="O66" s="440">
+      <c r="O66" s="444">
         <f t="shared" si="11"/>
         <v>0.08284</v>
       </c>
-      <c r="P66" s="440">
+      <c r="P66" s="444">
         <f t="shared" si="12"/>
         <v>3.1962775</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="3" t="s">
-        <v>767</v>
-      </c>
-      <c r="B67" s="447" t="s">
-        <v>768</v>
-      </c>
-      <c r="C67" s="442">
+        <v>776</v>
+      </c>
+      <c r="B67" s="451" t="s">
+        <v>777</v>
+      </c>
+      <c r="C67" s="446">
         <v>2.96</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>724</v>
+        <v>733</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>713</v>
+        <v>722</v>
       </c>
       <c r="F67" s="43">
         <v>100.0</v>
@@ -9511,38 +9548,38 @@
         <f t="shared" si="8"/>
         <v>104.4</v>
       </c>
-      <c r="M67" s="440">
+      <c r="M67" s="444">
         <f t="shared" si="9"/>
         <v>3.24</v>
       </c>
-      <c r="N67" s="440">
+      <c r="N67" s="444">
         <f t="shared" si="10"/>
         <v>0.0206625</v>
       </c>
-      <c r="O67" s="440">
+      <c r="O67" s="444">
         <f t="shared" si="11"/>
         <v>0.03477</v>
       </c>
-      <c r="P67" s="440">
+      <c r="P67" s="444">
         <f t="shared" si="12"/>
         <v>3.2954325</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="3" t="s">
-        <v>769</v>
-      </c>
-      <c r="B68" s="438" t="s">
-        <v>770</v>
-      </c>
-      <c r="C68" s="442">
+        <v>778</v>
+      </c>
+      <c r="B68" s="442" t="s">
+        <v>779</v>
+      </c>
+      <c r="C68" s="446">
         <v>1.59</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>771</v>
+        <v>780</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>713</v>
+        <v>722</v>
       </c>
       <c r="F68" s="43">
         <v>60.0</v>
@@ -9566,38 +9603,38 @@
         <f t="shared" si="8"/>
         <v>165.6</v>
       </c>
-      <c r="M68" s="440">
+      <c r="M68" s="444">
         <f t="shared" si="9"/>
         <v>4.14</v>
       </c>
-      <c r="N68" s="440">
+      <c r="N68" s="444">
         <f t="shared" si="10"/>
         <v>0.02565</v>
       </c>
-      <c r="O68" s="440">
+      <c r="O68" s="444">
         <f t="shared" si="11"/>
         <v>0.019</v>
       </c>
-      <c r="P68" s="440">
+      <c r="P68" s="444">
         <f t="shared" si="12"/>
         <v>4.18465</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="3" t="s">
-        <v>772</v>
-      </c>
-      <c r="B69" s="438" t="s">
-        <v>773</v>
-      </c>
-      <c r="C69" s="442">
+        <v>781</v>
+      </c>
+      <c r="B69" s="442" t="s">
+        <v>782</v>
+      </c>
+      <c r="C69" s="446">
         <v>0.772</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>774</v>
+        <v>783</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>713</v>
+        <v>722</v>
       </c>
       <c r="F69" s="43">
         <v>60.0</v>
@@ -9621,38 +9658,38 @@
         <f t="shared" si="8"/>
         <v>412.8</v>
       </c>
-      <c r="M69" s="440">
+      <c r="M69" s="444">
         <f t="shared" si="9"/>
         <v>4.32</v>
       </c>
-      <c r="N69" s="440">
+      <c r="N69" s="444">
         <f t="shared" si="10"/>
         <v>0.061275</v>
       </c>
-      <c r="O69" s="440">
+      <c r="O69" s="444">
         <f t="shared" si="11"/>
         <v>0.00684</v>
       </c>
-      <c r="P69" s="440">
+      <c r="P69" s="444">
         <f t="shared" si="12"/>
         <v>4.388115</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="3" t="s">
-        <v>775</v>
-      </c>
-      <c r="B70" s="441" t="s">
-        <v>776</v>
-      </c>
-      <c r="C70" s="442">
+        <v>784</v>
+      </c>
+      <c r="B70" s="445" t="s">
+        <v>785</v>
+      </c>
+      <c r="C70" s="446">
         <v>1.97</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>771</v>
+        <v>780</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>713</v>
+        <v>722</v>
       </c>
       <c r="F70" s="43">
         <v>100.0</v>
@@ -9676,38 +9713,38 @@
         <f t="shared" si="8"/>
         <v>196.1</v>
       </c>
-      <c r="M70" s="440">
+      <c r="M70" s="444">
         <f t="shared" si="9"/>
         <v>4.77</v>
       </c>
-      <c r="N70" s="440">
+      <c r="N70" s="444">
         <f t="shared" si="10"/>
         <v>0.0263625</v>
       </c>
-      <c r="O70" s="440">
+      <c r="O70" s="444">
         <f t="shared" si="11"/>
         <v>0.04294</v>
       </c>
-      <c r="P70" s="440">
+      <c r="P70" s="444">
         <f t="shared" si="12"/>
         <v>4.8393025</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="3" t="s">
-        <v>777</v>
-      </c>
-      <c r="B71" s="438" t="s">
-        <v>778</v>
-      </c>
-      <c r="C71" s="442">
+        <v>786</v>
+      </c>
+      <c r="B71" s="442" t="s">
+        <v>787</v>
+      </c>
+      <c r="C71" s="446">
         <v>0.725</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>779</v>
+        <v>788</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>713</v>
+        <v>722</v>
       </c>
       <c r="F71" s="43">
         <v>60.0</v>
@@ -9731,38 +9768,38 @@
         <f t="shared" si="8"/>
         <v>118.8</v>
       </c>
-      <c r="M71" s="440">
+      <c r="M71" s="444">
         <f t="shared" si="9"/>
         <v>4.86</v>
       </c>
-      <c r="N71" s="440">
+      <c r="N71" s="444">
         <f t="shared" si="10"/>
         <v>0.015675</v>
       </c>
-      <c r="O71" s="440">
+      <c r="O71" s="444">
         <f t="shared" si="11"/>
         <v>0.00532</v>
       </c>
-      <c r="P71" s="440">
+      <c r="P71" s="444">
         <f t="shared" si="12"/>
         <v>4.880995</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="3" t="s">
-        <v>780</v>
-      </c>
-      <c r="B72" s="447" t="s">
-        <v>781</v>
-      </c>
-      <c r="C72" s="442">
+        <v>789</v>
+      </c>
+      <c r="B72" s="451" t="s">
+        <v>790</v>
+      </c>
+      <c r="C72" s="446">
         <v>5.05</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>782</v>
+        <v>791</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>721</v>
+        <v>730</v>
       </c>
       <c r="F72" s="43">
         <v>100.0</v>
@@ -9786,38 +9823,38 @@
         <f t="shared" si="8"/>
         <v>50.6</v>
       </c>
-      <c r="M72" s="440">
+      <c r="M72" s="444">
         <f t="shared" si="9"/>
         <v>4.95</v>
       </c>
-      <c r="N72" s="440">
+      <c r="N72" s="444">
         <f t="shared" si="10"/>
         <v>0.006555</v>
       </c>
-      <c r="O72" s="440">
+      <c r="O72" s="444">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="P72" s="440">
+      <c r="P72" s="444">
         <f t="shared" si="12"/>
         <v>4.956555</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="7" t="s">
-        <v>783</v>
-      </c>
-      <c r="B73" s="448" t="s">
-        <v>784</v>
-      </c>
-      <c r="C73" s="442">
+        <v>792</v>
+      </c>
+      <c r="B73" s="452" t="s">
+        <v>793</v>
+      </c>
+      <c r="C73" s="446">
         <v>2.73</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>785</v>
+        <v>794</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>721</v>
+        <v>730</v>
       </c>
       <c r="F73" s="43">
         <v>150.0</v>
@@ -9841,38 +9878,38 @@
         <f t="shared" si="8"/>
         <v>42.56</v>
       </c>
-      <c r="M73" s="440">
+      <c r="M73" s="444">
         <f t="shared" si="9"/>
         <v>5.04</v>
       </c>
-      <c r="N73" s="440">
+      <c r="N73" s="444">
         <f t="shared" si="10"/>
         <v>0.005415</v>
       </c>
-      <c r="O73" s="440">
+      <c r="O73" s="444">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="P73" s="440">
+      <c r="P73" s="444">
         <f t="shared" si="12"/>
         <v>5.045415</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="7" t="s">
-        <v>786</v>
-      </c>
-      <c r="B74" s="447" t="s">
-        <v>787</v>
-      </c>
-      <c r="C74" s="442">
+        <v>795</v>
+      </c>
+      <c r="B74" s="451" t="s">
+        <v>796</v>
+      </c>
+      <c r="C74" s="446">
         <v>2.19</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>766</v>
+        <v>775</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>713</v>
+        <v>722</v>
       </c>
       <c r="F74" s="43">
         <v>100.0</v>
@@ -9896,38 +9933,38 @@
         <f t="shared" si="8"/>
         <v>246.4</v>
       </c>
-      <c r="M74" s="440">
+      <c r="M74" s="444">
         <f t="shared" si="9"/>
         <v>5.04</v>
       </c>
-      <c r="N74" s="440">
+      <c r="N74" s="444">
         <f t="shared" si="10"/>
         <v>0.03135</v>
       </c>
-      <c r="O74" s="440">
+      <c r="O74" s="444">
         <f t="shared" si="11"/>
         <v>0.06194</v>
       </c>
-      <c r="P74" s="440">
+      <c r="P74" s="444">
         <f t="shared" si="12"/>
         <v>5.13329</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="3" t="s">
-        <v>788</v>
-      </c>
-      <c r="B75" s="447" t="s">
-        <v>789</v>
-      </c>
-      <c r="C75" s="442">
+        <v>797</v>
+      </c>
+      <c r="B75" s="451" t="s">
+        <v>798</v>
+      </c>
+      <c r="C75" s="446">
         <v>8.3</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>790</v>
+        <v>799</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>721</v>
+        <v>730</v>
       </c>
       <c r="F75" s="43">
         <v>100.0</v>
@@ -9951,38 +9988,38 @@
         <f t="shared" si="8"/>
         <v>56</v>
       </c>
-      <c r="M75" s="440">
+      <c r="M75" s="444">
         <f t="shared" si="9"/>
         <v>6.3</v>
       </c>
-      <c r="N75" s="440">
+      <c r="N75" s="444">
         <f t="shared" si="10"/>
         <v>0.0057</v>
       </c>
-      <c r="O75" s="440">
+      <c r="O75" s="444">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="P75" s="440">
+      <c r="P75" s="444">
         <f t="shared" si="12"/>
         <v>6.3057</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="7" t="s">
-        <v>791</v>
-      </c>
-      <c r="B76" s="447" t="s">
-        <v>792</v>
-      </c>
-      <c r="C76" s="442">
+        <v>800</v>
+      </c>
+      <c r="B76" s="451" t="s">
+        <v>801</v>
+      </c>
+      <c r="C76" s="446">
         <v>3.26</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>766</v>
+        <v>775</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>713</v>
+        <v>722</v>
       </c>
       <c r="F76" s="43">
         <v>150.0</v>
@@ -10006,38 +10043,38 @@
         <f t="shared" si="8"/>
         <v>386.9</v>
       </c>
-      <c r="M76" s="440">
+      <c r="M76" s="444">
         <f t="shared" si="9"/>
         <v>6.57</v>
       </c>
-      <c r="N76" s="440">
+      <c r="N76" s="444">
         <f t="shared" si="10"/>
         <v>0.0377625</v>
       </c>
-      <c r="O76" s="440">
+      <c r="O76" s="444">
         <f t="shared" si="11"/>
         <v>0.04693</v>
       </c>
-      <c r="P76" s="440">
+      <c r="P76" s="444">
         <f t="shared" si="12"/>
         <v>6.6546925</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="7" t="s">
-        <v>793</v>
-      </c>
-      <c r="B77" s="447" t="s">
-        <v>794</v>
-      </c>
-      <c r="C77" s="442">
+        <v>802</v>
+      </c>
+      <c r="B77" s="451" t="s">
+        <v>803</v>
+      </c>
+      <c r="C77" s="446">
         <v>1.84</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>766</v>
+        <v>775</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>713</v>
+        <v>722</v>
       </c>
       <c r="F77" s="43">
         <v>100.0</v>
@@ -10061,38 +10098,38 @@
         <f t="shared" si="8"/>
         <v>292.6</v>
       </c>
-      <c r="M77" s="440">
+      <c r="M77" s="444">
         <f t="shared" si="9"/>
         <v>6.93</v>
       </c>
-      <c r="N77" s="440">
+      <c r="N77" s="444">
         <f t="shared" si="10"/>
         <v>0.027075</v>
       </c>
-      <c r="O77" s="440">
+      <c r="O77" s="444">
         <f t="shared" si="11"/>
         <v>0.0513</v>
       </c>
-      <c r="P77" s="440">
+      <c r="P77" s="444">
         <f t="shared" si="12"/>
         <v>7.008375</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="3" t="s">
-        <v>795</v>
-      </c>
-      <c r="B78" s="447" t="s">
-        <v>796</v>
-      </c>
-      <c r="C78" s="442">
+        <v>804</v>
+      </c>
+      <c r="B78" s="451" t="s">
+        <v>805</v>
+      </c>
+      <c r="C78" s="446">
         <v>4.61</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>797</v>
+        <v>806</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>798</v>
+        <v>807</v>
       </c>
       <c r="F78" s="43">
         <v>100.0</v>
@@ -10116,28 +10153,28 @@
         <f t="shared" si="8"/>
         <v>52.8</v>
       </c>
-      <c r="M78" s="440">
+      <c r="M78" s="444">
         <f t="shared" si="9"/>
         <v>14.4</v>
       </c>
-      <c r="N78" s="440">
+      <c r="N78" s="444">
         <f t="shared" si="10"/>
         <v>0.00235125</v>
       </c>
-      <c r="O78" s="440">
+      <c r="O78" s="444">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="P78" s="440">
+      <c r="P78" s="444">
         <f t="shared" si="12"/>
         <v>14.40235125</v>
       </c>
     </row>
     <row r="79">
-      <c r="C79" s="449"/>
+      <c r="C79" s="453"/>
     </row>
     <row r="80">
-      <c r="C80" s="449"/>
+      <c r="C80" s="453"/>
     </row>
   </sheetData>
   <autoFilter ref="$A$7:$M$35">
@@ -74820,6 +74857,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="2" max="2" width="13.5"/>
+    <col customWidth="1" min="6" max="6" width="18.38"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -75367,40 +75405,79 @@
         <f>20+C23*24</f>
         <v>128</v>
       </c>
+      <c r="F22" s="378" t="s">
+        <v>614</v>
+      </c>
+      <c r="G22" s="423"/>
+      <c r="H22" s="409"/>
     </row>
     <row r="23">
-      <c r="B23" s="423" t="s">
-        <v>614</v>
+      <c r="B23" s="424" t="s">
+        <v>615</v>
       </c>
       <c r="C23" s="391">
         <v>4.5</v>
       </c>
-      <c r="D23" s="424" t="s">
-        <v>615</v>
+      <c r="D23" s="425" t="s">
+        <v>616</v>
+      </c>
+      <c r="F23" s="415" t="s">
+        <v>617</v>
+      </c>
+      <c r="G23" s="391">
+        <v>166.3</v>
+      </c>
+      <c r="H23" s="414" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="24">
-      <c r="B24" s="425" t="s">
-        <v>616</v>
+      <c r="B24" s="426" t="s">
+        <v>618</v>
       </c>
       <c r="C24" s="400">
         <f>IF(D22&lt;120,120,D22)</f>
         <v>128</v>
       </c>
-      <c r="D24" s="426" t="s">
+      <c r="D24" s="427" t="s">
         <v>120</v>
       </c>
+      <c r="F24" s="415" t="s">
+        <v>619</v>
+      </c>
+      <c r="G24" s="391">
+        <v>56.2</v>
+      </c>
+      <c r="H24" s="414" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="F25" s="428" t="s">
+        <v>620</v>
+      </c>
+      <c r="G25" s="88">
+        <v>28.0</v>
+      </c>
+      <c r="H25" s="429"/>
     </row>
     <row r="26">
       <c r="B26" s="378" t="s">
-        <v>617</v>
+        <v>621</v>
       </c>
       <c r="C26" s="408"/>
       <c r="D26" s="409"/>
+      <c r="F26" s="428" t="s">
+        <v>622</v>
+      </c>
+      <c r="G26" s="88">
+        <v>2.0</v>
+      </c>
+      <c r="H26" s="429"/>
     </row>
     <row r="27">
       <c r="B27" s="415" t="s">
-        <v>618</v>
+        <v>623</v>
       </c>
       <c r="C27" s="395">
         <v>92.2</v>
@@ -75408,10 +75485,18 @@
       <c r="D27" s="414" t="s">
         <v>227</v>
       </c>
+      <c r="F27" s="415" t="s">
+        <v>624</v>
+      </c>
+      <c r="G27" s="386">
+        <f>G25/G26</f>
+        <v>14</v>
+      </c>
+      <c r="H27" s="414"/>
     </row>
     <row r="28">
       <c r="B28" s="415" t="s">
-        <v>619</v>
+        <v>625</v>
       </c>
       <c r="C28" s="395">
         <v>1.0</v>
@@ -75419,19 +75504,37 @@
       <c r="D28" s="414" t="s">
         <v>227</v>
       </c>
+      <c r="F28" s="415" t="s">
+        <v>626</v>
+      </c>
+      <c r="G28" s="430">
+        <f>SQRT(1-(G24/G23))</f>
+        <v>0.8136685593</v>
+      </c>
+      <c r="H28" s="414"/>
     </row>
     <row r="29">
       <c r="B29" s="415" t="s">
-        <v>620</v>
+        <v>627</v>
       </c>
       <c r="C29" s="395">
         <v>1650.0</v>
       </c>
       <c r="D29" s="414"/>
+      <c r="F29" s="415" t="s">
+        <v>628</v>
+      </c>
+      <c r="G29" s="430">
+        <f>G23/G27^2</f>
+        <v>0.8484693878</v>
+      </c>
+      <c r="H29" s="414" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="30">
       <c r="B30" s="415" t="s">
-        <v>621</v>
+        <v>629</v>
       </c>
       <c r="C30" s="395">
         <v>125.0</v>
@@ -75439,10 +75542,18 @@
       <c r="D30" s="414" t="s">
         <v>608</v>
       </c>
+      <c r="F30" s="418" t="s">
+        <v>630</v>
+      </c>
+      <c r="G30" s="419">
+        <f>G23/G24</f>
+        <v>2.959074733</v>
+      </c>
+      <c r="H30" s="420"/>
     </row>
     <row r="31">
       <c r="B31" s="415" t="s">
-        <v>622</v>
+        <v>631</v>
       </c>
       <c r="C31" s="395">
         <v>28.0</v>
@@ -75451,7 +75562,7 @@
     </row>
     <row r="32">
       <c r="B32" s="415" t="s">
-        <v>623</v>
+        <v>632</v>
       </c>
       <c r="C32" s="394">
         <f>C31^2/(C33*10^-6)</f>
@@ -75463,14 +75574,14 @@
     </row>
     <row r="33">
       <c r="B33" s="418" t="s">
-        <v>624</v>
+        <v>633</v>
       </c>
       <c r="C33" s="400">
         <f>(((C27-C28)/1000)/(4*pi()*10^-7*C29*C30*10^-6))+((C28/1000)/(4*pi()*10^-7*1*C30*10^-6))</f>
         <v>6718074.834</v>
       </c>
-      <c r="D33" s="427" t="s">
-        <v>625</v>
+      <c r="D33" s="431" t="s">
+        <v>634</v>
       </c>
     </row>
   </sheetData>

</xml_diff>